<commit_message>
touch ups and a couple images
</commit_message>
<xml_diff>
--- a/bottlenecks.xlsx
+++ b/bottlenecks.xlsx
@@ -19,7 +19,7 @@
     <definedName name="bandwidth1">'Current Bitcoin'!$B$44</definedName>
     <definedName name="bandwidth10">'Future Bitcoin'!$B$36</definedName>
     <definedName name="bandwidth13">'Future Bitcoin'!#REF!</definedName>
-    <definedName name="bandwidth15">'Future Bitcoin'!$B$119</definedName>
+    <definedName name="bandwidth15">'Future Bitcoin'!$B$120</definedName>
     <definedName name="bandwidth2">'Current Bitcoin'!$B$68</definedName>
     <definedName name="bandwidth3">'Current Bitcoin'!$B$92</definedName>
     <definedName name="bandwidth4">'Future Bitcoin'!#REF!</definedName>
@@ -36,9 +36,9 @@
     <definedName name="disk6">'Current Bitcoin'!$C$228</definedName>
     <definedName name="disk7">'Current Bitcoin'!$C$252</definedName>
     <definedName name="diskGrowth">'Current Bitcoin'!$C$6</definedName>
-    <definedName name="endGameEmergencyUsage">'Future Bitcoin'!$G$124</definedName>
-    <definedName name="endGameTransactionSize">'Future Bitcoin'!$A$124</definedName>
-    <definedName name="endGameUsers">'Future Bitcoin'!$C$124</definedName>
+    <definedName name="endGameEmergencyUsage">'Future Bitcoin'!$G$125</definedName>
+    <definedName name="endGameTransactionSize">'Future Bitcoin'!$A$125</definedName>
+    <definedName name="endGameUsers">'Future Bitcoin'!$C$125</definedName>
     <definedName name="historicalResourcePercent10">'Future Bitcoin'!$L$36</definedName>
     <definedName name="historicalResourcePercent12">'Future Bitcoin'!$L$84</definedName>
     <definedName name="historicalResourcePercent13">'Future Bitcoin'!#REF!</definedName>
@@ -51,7 +51,7 @@
     <definedName name="KBperGB">'Current Bitcoin'!$E$10</definedName>
     <definedName name="mbToGB">'Current Bitcoin'!$D$10</definedName>
     <definedName name="memory1">'Current Bitcoin'!$D$44</definedName>
-    <definedName name="memory15">'Future Bitcoin'!$D$119</definedName>
+    <definedName name="memory15">'Future Bitcoin'!$D$120</definedName>
     <definedName name="memory2">'Current Bitcoin'!$D$68</definedName>
     <definedName name="memory3">'Current Bitcoin'!$D$92</definedName>
     <definedName name="memory6">'Current Bitcoin'!$D$228</definedName>
@@ -61,7 +61,7 @@
     <definedName name="ongoingResourcePercent6">'Current Bitcoin'!$K$228</definedName>
     <definedName name="ongoingResourcePercent6p5">'Current Bitcoin'!$K$277</definedName>
     <definedName name="ongoingResourcePercent7">'Current Bitcoin'!$K$252</definedName>
-    <definedName name="ongoingResourcePercentage15">'Future Bitcoin'!$L$119</definedName>
+    <definedName name="ongoingResourcePercentage15">'Future Bitcoin'!$L$120</definedName>
     <definedName name="ongoingResourcePercentage4">'Future Bitcoin'!#REF!</definedName>
     <definedName name="ongoingResourcePercentage5">'Current Bitcoin'!$K$204</definedName>
     <definedName name="ongoingResourcePercentage8">'Current Bitcoin'!$K$156</definedName>
@@ -73,7 +73,7 @@
     <definedName name="publicConnections9">'Current Bitcoin'!$H$180</definedName>
     <definedName name="publicNodePercent">'Current Bitcoin'!$F$15</definedName>
     <definedName name="recentSyncTime11">'Future Bitcoin'!$I$60</definedName>
-    <definedName name="recentSyncTime15">'Future Bitcoin'!$I$119</definedName>
+    <definedName name="recentSyncTime15">'Future Bitcoin'!$I$120</definedName>
     <definedName name="recentSyncTime8">'Future Bitcoin'!$I$12</definedName>
     <definedName name="resourcePercent">'Current Bitcoin'!$J$44</definedName>
     <definedName name="resourcePercent2">'Current Bitcoin'!$J$68</definedName>
@@ -83,7 +83,7 @@
     <definedName name="syncResourcePercent10">'Future Bitcoin'!$K$36</definedName>
     <definedName name="syncResourcePercent11">'Future Bitcoin'!$K$60</definedName>
     <definedName name="syncResourcePercent8">'Future Bitcoin'!$K$12</definedName>
-    <definedName name="syncResourcePercentage15">'Future Bitcoin'!$K$119</definedName>
+    <definedName name="syncResourcePercentage15">'Future Bitcoin'!$K$120</definedName>
     <definedName name="syncTime1">'Current Bitcoin'!$I$44</definedName>
     <definedName name="syncTime2">'Current Bitcoin'!$I$68</definedName>
     <definedName name="syncTime3">'Current Bitcoin'!$I$92</definedName>
@@ -100,7 +100,7 @@
     <definedName name="utxoGrowth">'Current Bitcoin'!$E$19</definedName>
     <definedName name="utxoMemoryPercent">'Current Bitcoin'!$D$15</definedName>
     <definedName name="utxoSize">'Current Bitcoin'!$D$19</definedName>
-    <definedName name="utxosPerUserEndGame">'Future Bitcoin'!$D$124</definedName>
+    <definedName name="utxosPerUserEndGame">'Future Bitcoin'!$D$125</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="135">
   <si>
     <t>User Type</t>
   </si>
@@ -448,9 +448,6 @@
     <t>Ongoing Transaction Download &amp; Upload (10th %ile)</t>
   </si>
   <si>
-    <t>End Game</t>
-  </si>
-  <si>
     <t>TPS</t>
   </si>
   <si>
@@ -530,6 +527,15 @@
   </si>
   <si>
     <t>Initial Sync</t>
+  </si>
+  <si>
+    <t>Future throughput</t>
+  </si>
+  <si>
+    <t>Future throughput summary (based on today)</t>
+  </si>
+  <si>
+    <t>Future throughput summary (based on 10 years from now)</t>
   </si>
 </sst>
 </file>
@@ -936,7 +942,58 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBD1D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBD1D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBD1D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1002,6 +1059,30 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBD1D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1190,8 +1271,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146995072"/>
-        <c:axId val="147001344"/>
+        <c:axId val="146687872"/>
+        <c:axId val="146690048"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1339,11 +1420,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147004416"/>
-        <c:axId val="147002880"/>
+        <c:axId val="146693120"/>
+        <c:axId val="146691584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146995072"/>
+        <c:axId val="146687872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1365,14 +1446,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147001344"/>
+        <c:crossAx val="146690048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1380,7 +1460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147001344"/>
+        <c:axId val="146690048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,12 +1485,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146995072"/>
+        <c:crossAx val="146687872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147002880"/>
+        <c:axId val="146691584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1436,12 +1516,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147004416"/>
+        <c:crossAx val="146693120"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="147004416"/>
+        <c:axId val="146693120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147002880"/>
+        <c:crossAx val="146691584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1658,8 +1738,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147047168"/>
-        <c:axId val="147049088"/>
+        <c:axId val="146719488"/>
+        <c:axId val="146721408"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1807,11 +1887,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147060608"/>
-        <c:axId val="147059072"/>
+        <c:axId val="146728832"/>
+        <c:axId val="146727296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147047168"/>
+        <c:axId val="146719488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,14 +1913,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147049088"/>
+        <c:crossAx val="146721408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1848,7 +1927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147049088"/>
+        <c:axId val="146721408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,12 +1952,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147047168"/>
+        <c:crossAx val="146719488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147059072"/>
+        <c:axId val="146727296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1904,12 +1983,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147060608"/>
+        <c:crossAx val="146728832"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="147060608"/>
+        <c:axId val="146728832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1919,7 +1998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147059072"/>
+        <c:crossAx val="146727296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2126,8 +2205,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147086720"/>
-        <c:axId val="147092992"/>
+        <c:axId val="147283328"/>
+        <c:axId val="147293696"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2275,11 +2354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147104512"/>
-        <c:axId val="147094528"/>
+        <c:axId val="147305216"/>
+        <c:axId val="147295232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147086720"/>
+        <c:axId val="147283328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2301,14 +2380,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147092992"/>
+        <c:crossAx val="147293696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2316,7 +2394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147092992"/>
+        <c:axId val="147293696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2341,12 +2419,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147086720"/>
+        <c:crossAx val="147283328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147094528"/>
+        <c:axId val="147295232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2372,12 +2450,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147104512"/>
+        <c:crossAx val="147305216"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="147104512"/>
+        <c:axId val="147305216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,7 +2465,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147094528"/>
+        <c:crossAx val="147295232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2595,8 +2673,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163126272"/>
-        <c:axId val="163132544"/>
+        <c:axId val="147397632"/>
+        <c:axId val="147403904"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2744,11 +2822,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163148160"/>
-        <c:axId val="163134080"/>
+        <c:axId val="147419520"/>
+        <c:axId val="147405440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163126272"/>
+        <c:axId val="147397632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2770,14 +2848,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163132544"/>
+        <c:crossAx val="147403904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2785,7 +2862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163132544"/>
+        <c:axId val="147403904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2810,12 +2887,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163126272"/>
+        <c:crossAx val="147397632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="163134080"/>
+        <c:axId val="147405440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,12 +2918,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163148160"/>
+        <c:crossAx val="147419520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="163148160"/>
+        <c:axId val="147419520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,7 +2933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163134080"/>
+        <c:crossAx val="147405440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3211,11 +3288,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163175424"/>
-        <c:axId val="163181696"/>
+        <c:axId val="147446400"/>
+        <c:axId val="147448576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163175424"/>
+        <c:axId val="147446400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3237,13 +3314,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163181696"/>
+        <c:crossAx val="147448576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3251,7 +3329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163181696"/>
+        <c:axId val="147448576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3276,7 +3354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163175424"/>
+        <c:crossAx val="147446400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3481,8 +3559,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163208192"/>
-        <c:axId val="163226752"/>
+        <c:axId val="147487744"/>
+        <c:axId val="147494016"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3630,11 +3708,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163230080"/>
-        <c:axId val="163228288"/>
+        <c:axId val="147505536"/>
+        <c:axId val="147495552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163208192"/>
+        <c:axId val="147487744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3662,7 +3740,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163226752"/>
+        <c:crossAx val="147494016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3670,7 +3748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163226752"/>
+        <c:axId val="147494016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3695,12 +3773,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163208192"/>
+        <c:crossAx val="147487744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="163228288"/>
+        <c:axId val="147495552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,12 +3804,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163230080"/>
+        <c:crossAx val="147505536"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="163230080"/>
+        <c:axId val="147505536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3741,7 +3819,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163228288"/>
+        <c:crossAx val="147495552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4095,11 +4173,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163240960"/>
-        <c:axId val="163337344"/>
+        <c:axId val="147516032"/>
+        <c:axId val="147604224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163240960"/>
+        <c:axId val="147516032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4127,7 +4205,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163337344"/>
+        <c:crossAx val="147604224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4135,7 +4213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163337344"/>
+        <c:axId val="147604224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4160,7 +4238,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163240960"/>
+        <c:crossAx val="147516032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4365,11 +4443,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="162333824"/>
-        <c:axId val="162335744"/>
+        <c:axId val="147129472"/>
+        <c:axId val="147131392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="162333824"/>
+        <c:axId val="147129472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4391,14 +4469,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162335744"/>
+        <c:crossAx val="147131392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4406,7 +4483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162335744"/>
+        <c:axId val="147131392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4433,7 +4510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162333824"/>
+        <c:crossAx val="147129472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5336,8 +5413,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K309"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="A4:K4"/>
+    <sheetView topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="D309" sqref="D309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5704,7 +5781,7 @@
     </row>
     <row r="21" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -10744,63 +10821,63 @@
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="147" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B306" s="147"/>
       <c r="C306" s="147"/>
       <c r="D306" s="2" t="str">
-        <f>A204</f>
+        <f>A156</f>
         <v>90th %ile</v>
       </c>
       <c r="E306" s="45">
-        <f>B208</f>
-        <v>20</v>
-      </c>
-      <c r="F306" s="13">
-        <f>C208*1000</f>
-        <v>5700</v>
-      </c>
-      <c r="G306" s="56"/>
+        <f>D160</f>
+        <v>10.096930533117932</v>
+      </c>
+      <c r="F306" s="9">
+        <f>E160*1000</f>
+        <v>2877.6252019386106</v>
+      </c>
+      <c r="G306" s="57"/>
       <c r="H306" s="132"/>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="147" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B307" s="147"/>
       <c r="C307" s="147"/>
       <c r="D307" s="2" t="str">
-        <f>A228</f>
+        <f>A204</f>
         <v>90th %ile</v>
       </c>
-      <c r="E307" s="58"/>
-      <c r="F307" s="57"/>
+      <c r="E307" s="45">
+        <f>B208</f>
+        <v>20</v>
+      </c>
+      <c r="F307" s="13">
+        <f>C208*1000</f>
+        <v>5700</v>
+      </c>
       <c r="G307" s="56"/>
-      <c r="H307" s="54">
-        <f>B232</f>
-        <v>12.8</v>
-      </c>
+      <c r="H307" s="132"/>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="147" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B308" s="147"/>
       <c r="C308" s="147"/>
       <c r="D308" s="2" t="str">
-        <f>A156</f>
+        <f>A228</f>
         <v>90th %ile</v>
       </c>
-      <c r="E308" s="45">
-        <f>D160</f>
-        <v>10.096930533117932</v>
-      </c>
-      <c r="F308" s="9">
-        <f>E160*1000</f>
-        <v>2877.6252019386106</v>
-      </c>
-      <c r="G308" s="57"/>
-      <c r="H308" s="132"/>
+      <c r="E308" s="58"/>
+      <c r="F308" s="57"/>
+      <c r="G308" s="56"/>
+      <c r="H308" s="54">
+        <f>B232</f>
+        <v>12.8</v>
+      </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="147" t="s">
@@ -10808,9 +10885,8 @@
       </c>
       <c r="B309" s="147"/>
       <c r="C309" s="147"/>
-      <c r="D309" s="110">
-        <f>A258</f>
-        <v>2</v>
+      <c r="D309" s="110" t="s">
+        <v>85</v>
       </c>
       <c r="E309" s="46">
         <f>D184</f>
@@ -10826,15 +10902,15 @@
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A300:C300"/>
-    <mergeCell ref="A307:C307"/>
+    <mergeCell ref="A308:C308"/>
     <mergeCell ref="A309:C309"/>
     <mergeCell ref="A302:C302"/>
     <mergeCell ref="A301:C301"/>
     <mergeCell ref="A305:C305"/>
-    <mergeCell ref="A306:C306"/>
+    <mergeCell ref="A307:C307"/>
     <mergeCell ref="A304:C304"/>
     <mergeCell ref="A303:C303"/>
-    <mergeCell ref="A308:C308"/>
+    <mergeCell ref="A306:C306"/>
   </mergeCells>
   <conditionalFormatting sqref="I117:I132">
     <cfRule type="colorScale" priority="8">
@@ -10860,23 +10936,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F301:F303 F308 F305:F306">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="F301:F303 F305:F307">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
       <formula>$C$19</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E301:E303 E308 E305:E306">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="E301:E303 E305:E307">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>$C$19*1000/$C$10/$F$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G301:G303 G305">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
       <formula>$B$19</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H307 H304">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="H308 H304">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>$D$19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10889,10 +10965,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L194"/>
+  <dimension ref="A1:L207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="I136" sqref="I136"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="I208" sqref="I208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13366,1371 +13442,1597 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="113" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" s="110" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="113"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="110" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:12" s="108" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="110" t="s">
+    <row r="120" spans="1:12" s="108" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="B119" s="115">
+      <c r="B120" s="115">
         <v>50</v>
       </c>
-      <c r="C119" s="116">
+      <c r="C120" s="116">
         <v>1000</v>
       </c>
-      <c r="D119" s="116">
+      <c r="D120" s="116">
         <v>8</v>
       </c>
-      <c r="E119" s="117">
+      <c r="E120" s="117">
         <v>5000</v>
       </c>
-      <c r="F119" s="118" t="s">
+      <c r="F120" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="G119" s="121">
+      <c r="G120" s="121">
         <v>8</v>
       </c>
-      <c r="H119" s="133">
+      <c r="H120" s="133">
         <f>($G$5*0.9+$G$4*0.09+$G$3*0.01)/publicNodePercent</f>
         <v>80</v>
       </c>
-      <c r="I119" s="119">
+      <c r="I120" s="119">
         <v>7</v>
       </c>
-      <c r="J119" s="119">
+      <c r="J120" s="119">
         <v>60</v>
       </c>
-      <c r="K119" s="120">
+      <c r="K120" s="120">
         <f>'Current Bitcoin'!$J$4</f>
         <v>0.5</v>
       </c>
-      <c r="L119" s="120">
+      <c r="L120" s="120">
         <v>0.1</v>
       </c>
     </row>
-    <row r="120" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G121" s="109" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" s="109" t="s">
-        <v>123</v>
-      </c>
-      <c r="B122" s="109" t="s">
-        <v>124</v>
-      </c>
-      <c r="C122" s="109"/>
-      <c r="D122" s="109" t="s">
-        <v>110</v>
-      </c>
-      <c r="E122" s="109" t="s">
-        <v>117</v>
-      </c>
-      <c r="F122" s="109" t="s">
-        <v>115</v>
-      </c>
+    <row r="121" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G122" s="109" t="s">
-        <v>120</v>
-      </c>
-      <c r="H122" s="109"/>
+        <v>118</v>
+      </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="109" t="s">
         <v>122</v>
       </c>
       <c r="B123" s="109" t="s">
-        <v>122</v>
-      </c>
-      <c r="C123" s="109" t="s">
+        <v>123</v>
+      </c>
+      <c r="C123" s="109"/>
+      <c r="D123" s="109" t="s">
         <v>109</v>
-      </c>
-      <c r="D123" s="109" t="s">
-        <v>111</v>
       </c>
       <c r="E123" s="109" t="s">
         <v>116</v>
       </c>
       <c r="F123" s="109" t="s">
+        <v>114</v>
+      </c>
+      <c r="G123" s="109" t="s">
+        <v>119</v>
+      </c>
+      <c r="H123" s="109"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="B124" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="C124" s="109" t="s">
+        <v>108</v>
+      </c>
+      <c r="D124" s="109" t="s">
+        <v>110</v>
+      </c>
+      <c r="E124" s="109" t="s">
+        <v>115</v>
+      </c>
+      <c r="F124" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="G123" s="109" t="s">
-        <v>121</v>
-      </c>
-      <c r="H123" s="109"/>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A124" s="23">
+      <c r="G124" s="109" t="s">
+        <v>120</v>
+      </c>
+      <c r="H124" s="109"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="23">
         <f>avgTrSize</f>
         <v>475</v>
       </c>
-      <c r="B124" s="121">
+      <c r="B125" s="121">
         <v>2</v>
       </c>
-      <c r="C124" s="140">
+      <c r="C125" s="140">
         <v>8</v>
       </c>
-      <c r="D124" s="121">
+      <c r="D125" s="121">
         <v>100</v>
       </c>
-      <c r="E124" s="142">
+      <c r="E125" s="142">
         <v>1E-4</v>
       </c>
-      <c r="F124">
-        <f>CEILING(LOG(E124,0.5),1)</f>
+      <c r="F125">
+        <f>CEILING(LOG(E125,0.5),1)</f>
         <v>14</v>
       </c>
-      <c r="G124" s="143">
+      <c r="G125" s="143">
         <v>0.75</v>
       </c>
-      <c r="I124" s="108"/>
-    </row>
-    <row r="126" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="113" t="s">
-        <v>132</v>
-      </c>
+      <c r="I125" s="108"/>
     </row>
     <row r="127" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="109"/>
-      <c r="C127" s="109" t="s">
+      <c r="A127" s="113" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="109"/>
+      <c r="C128" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="D127" s="109" t="s">
+      <c r="D128" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="E127" s="109" t="s">
+      <c r="E128" s="109" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:12" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="145" t="s">
+    <row r="129" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="B128" s="109" t="s">
+      <c r="B129" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="C128" s="109" t="s">
+      <c r="C129" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="D128" s="109" t="s">
+      <c r="D129" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="E128" s="109" t="s">
+      <c r="E129" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="F128" s="109" t="s">
+      <c r="F129" s="109" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="108">
+    <row r="130" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="108">
         <v>0</v>
       </c>
-      <c r="B129" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A129)*recentSyncTime15/365</f>
+      <c r="B130" s="130">
+        <f t="shared" ref="B130:B145" si="19">bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A130)*recentSyncTime15/365</f>
         <v>1890</v>
       </c>
-      <c r="C129" s="102">
+      <c r="C130" s="102">
         <f xml:space="preserve"> utxoSize</f>
         <v>3</v>
       </c>
-      <c r="D129" s="114">
-        <f>(B129-C129)/(assumevalidBlockTime/365)</f>
+      <c r="D130" s="114">
+        <f>(B130-C130)/(assumevalidBlockTime/365)</f>
         <v>3279.7857142857147</v>
       </c>
-      <c r="E129" s="129">
-        <f>(D129*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
+      <c r="E130" s="129">
+        <f>(D130*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
         <v>62.400793650793652</v>
       </c>
-      <c r="F129" s="93">
-        <f t="shared" ref="F129:F144" si="19">E129*1000*1000/(secondsPerBlock*avgTrSize)</f>
+      <c r="F130" s="93">
+        <f t="shared" ref="F130:F145" si="20">E130*1000*1000/(secondsPerBlock*avgTrSize)</f>
         <v>218.95015316067949</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="108">
-        <v>1</v>
-      </c>
-      <c r="B130" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A130)*recentSyncTime15/365</f>
-        <v>2362.5</v>
-      </c>
-      <c r="C130" s="104">
-        <f xml:space="preserve"> C129 + MIN(C129*utxoGrowth, curMaxBlocksize*secondsPerYear/secondsPerBlock/KBperGB)</f>
-        <v>4.5</v>
-      </c>
-      <c r="D130" s="114">
-        <f t="shared" ref="D129:D144" si="20">(B130-C130)/(assumevalidBlockTime/365)</f>
-        <v>4098.4285714285716</v>
-      </c>
-      <c r="E130" s="129">
-        <f t="shared" ref="E129:E131" si="21">(D130*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
-        <v>77.976190476190482</v>
-      </c>
-      <c r="F130" s="93">
-        <f t="shared" si="19"/>
-        <v>273.60066833751051</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B131" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A131)*recentSyncTime15/365</f>
-        <v>2953.125</v>
+        <f t="shared" si="19"/>
+        <v>2362.5</v>
       </c>
       <c r="C131" s="104">
-        <f t="shared" ref="C130:C144" si="22" xml:space="preserve"> C130 + MIN(C130*utxoGrowth, curMaxBlocksize*secondsPerYear/secondsPerBlock/KBperGB)</f>
-        <v>6.75</v>
+        <f xml:space="preserve"> C130 + MIN(C130*utxoGrowth, curMaxBlocksize*secondsPerYear/secondsPerBlock/KBperGB)</f>
+        <v>4.5</v>
       </c>
       <c r="D131" s="114">
+        <f t="shared" ref="D131:D145" si="21">(B131-C131)/(assumevalidBlockTime/365)</f>
+        <v>4098.4285714285716</v>
+      </c>
+      <c r="E131" s="129">
+        <f t="shared" ref="E131:E132" si="22">(D131*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
+        <v>77.976190476190482</v>
+      </c>
+      <c r="F131" s="93">
         <f t="shared" si="20"/>
-        <v>5121.0803571428578</v>
-      </c>
-      <c r="E131" s="129">
-        <f t="shared" si="21"/>
-        <v>97.433035714285708</v>
-      </c>
-      <c r="F131" s="93">
-        <f t="shared" si="19"/>
-        <v>341.87030075187971</v>
+        <v>273.60066833751051</v>
       </c>
     </row>
     <row r="132" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="108">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B132" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A132)*recentSyncTime15/365</f>
-        <v>3691.40625</v>
+        <f t="shared" si="19"/>
+        <v>2953.125</v>
       </c>
       <c r="C132" s="104">
+        <f t="shared" ref="C132:C145" si="23" xml:space="preserve"> C131 + MIN(C131*utxoGrowth, curMaxBlocksize*secondsPerYear/secondsPerBlock/KBperGB)</f>
+        <v>6.75</v>
+      </c>
+      <c r="D132" s="114">
+        <f t="shared" si="21"/>
+        <v>5121.0803571428578</v>
+      </c>
+      <c r="E132" s="129">
         <f t="shared" si="22"/>
-        <v>10.125</v>
-      </c>
-      <c r="D132" s="114">
+        <v>97.433035714285708</v>
+      </c>
+      <c r="F132" s="93">
         <f t="shared" si="20"/>
-        <v>6398.4174107142862</v>
-      </c>
-      <c r="E132" s="129">
-        <f>(D132*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
-        <v>121.73549107142857</v>
-      </c>
-      <c r="F132" s="93">
-        <f t="shared" si="19"/>
-        <v>427.14207393483707</v>
+        <v>341.87030075187971</v>
       </c>
     </row>
     <row r="133" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B133" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A133)*recentSyncTime15/365</f>
-        <v>4614.2578125</v>
+        <f t="shared" si="19"/>
+        <v>3691.40625</v>
       </c>
       <c r="C133" s="104">
-        <f t="shared" si="22"/>
-        <v>15.1875</v>
+        <f t="shared" si="23"/>
+        <v>10.125</v>
       </c>
       <c r="D133" s="114">
+        <f t="shared" si="21"/>
+        <v>6398.4174107142862</v>
+      </c>
+      <c r="E133" s="129">
+        <f>(D133*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
+        <v>121.73549107142857</v>
+      </c>
+      <c r="F133" s="93">
         <f t="shared" si="20"/>
-        <v>7993.6222098214294</v>
-      </c>
-      <c r="E133" s="129">
-        <f t="shared" ref="E133:E144" si="23">(D133*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
-        <v>152.08565848214286</v>
-      </c>
-      <c r="F133" s="93">
-        <f t="shared" si="19"/>
-        <v>533.63388941102755</v>
+        <v>427.14207393483707</v>
       </c>
     </row>
     <row r="134" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="108">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B134" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A134)*recentSyncTime15/365</f>
-        <v>5767.822265625</v>
+        <f t="shared" si="19"/>
+        <v>4614.2578125</v>
       </c>
       <c r="C134" s="104">
-        <f t="shared" si="22"/>
-        <v>22.78125</v>
+        <f t="shared" si="23"/>
+        <v>15.1875</v>
       </c>
       <c r="D134" s="114">
+        <f t="shared" si="21"/>
+        <v>7993.6222098214294</v>
+      </c>
+      <c r="E134" s="129">
+        <f t="shared" ref="E134:E145" si="24">(D134*KBperGB/secondsPerYear)*secondsPerBlock/1000</f>
+        <v>152.08565848214286</v>
+      </c>
+      <c r="F134" s="93">
         <f t="shared" si="20"/>
-        <v>9985.4284319196431</v>
-      </c>
-      <c r="E134" s="129">
-        <f t="shared" si="23"/>
-        <v>189.98151506696428</v>
-      </c>
-      <c r="F134" s="93">
-        <f t="shared" si="19"/>
-        <v>666.60180725250632</v>
+        <v>533.63388941102755</v>
       </c>
     </row>
     <row r="135" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="108">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B135" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A135)*recentSyncTime15/365</f>
-        <v>7209.77783203125</v>
+        <f t="shared" si="19"/>
+        <v>5767.822265625</v>
       </c>
       <c r="C135" s="104">
-        <f t="shared" si="22"/>
-        <v>34.171875</v>
+        <f t="shared" si="23"/>
+        <v>22.78125</v>
       </c>
       <c r="D135" s="114">
+        <f t="shared" si="21"/>
+        <v>9985.4284319196431</v>
+      </c>
+      <c r="E135" s="129">
+        <f t="shared" si="24"/>
+        <v>189.98151506696428</v>
+      </c>
+      <c r="F135" s="93">
         <f t="shared" si="20"/>
-        <v>12471.886544363841</v>
-      </c>
-      <c r="E135" s="129">
-        <f t="shared" si="23"/>
-        <v>237.28855678013394</v>
-      </c>
-      <c r="F135" s="93">
-        <f t="shared" si="19"/>
-        <v>832.59142729871564</v>
+        <v>666.60180725250632</v>
       </c>
     </row>
     <row r="136" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="108">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B136" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A136)*recentSyncTime15/365</f>
-        <v>9012.2222900390625</v>
+        <f t="shared" si="19"/>
+        <v>7209.77783203125</v>
       </c>
       <c r="C136" s="104">
-        <f t="shared" si="22"/>
-        <v>51.2578125</v>
+        <f t="shared" si="23"/>
+        <v>34.171875</v>
       </c>
       <c r="D136" s="114">
+        <f t="shared" si="21"/>
+        <v>12471.886544363841</v>
+      </c>
+      <c r="E136" s="129">
+        <f t="shared" si="24"/>
+        <v>237.28855678013394</v>
+      </c>
+      <c r="F136" s="93">
         <f t="shared" si="20"/>
-        <v>15575.009687151229</v>
-      </c>
-      <c r="E136" s="129">
-        <f t="shared" si="23"/>
-        <v>296.32819039481029</v>
-      </c>
-      <c r="F136" s="93">
-        <f t="shared" si="19"/>
-        <v>1039.7480364730184</v>
+        <v>832.59142729871564</v>
       </c>
     </row>
     <row r="137" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="108">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B137" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A137)*recentSyncTime15/365</f>
-        <v>11265.277862548828</v>
+        <f t="shared" si="19"/>
+        <v>9012.2222900390625</v>
       </c>
       <c r="C137" s="104">
-        <f t="shared" si="22"/>
-        <v>76.88671875</v>
+        <f t="shared" si="23"/>
+        <v>51.2578125</v>
       </c>
       <c r="D137" s="114">
+        <f t="shared" si="21"/>
+        <v>15575.009687151229</v>
+      </c>
+      <c r="E137" s="129">
+        <f t="shared" si="24"/>
+        <v>296.32819039481029</v>
+      </c>
+      <c r="F137" s="93">
         <f t="shared" si="20"/>
-        <v>19446.489368983679</v>
-      </c>
-      <c r="E137" s="129">
-        <f t="shared" si="23"/>
-        <v>369.98647962297719</v>
-      </c>
-      <c r="F137" s="93">
-        <f t="shared" si="19"/>
-        <v>1298.1981741157094</v>
+        <v>1039.7480364730184</v>
       </c>
     </row>
     <row r="138" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="108">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B138" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A138)*recentSyncTime15/365</f>
-        <v>14081.597328186035</v>
+        <f t="shared" si="19"/>
+        <v>11265.277862548828</v>
       </c>
       <c r="C138" s="104">
-        <f t="shared" si="22"/>
-        <v>115.330078125</v>
+        <f t="shared" si="23"/>
+        <v>76.88671875</v>
       </c>
       <c r="D138" s="114">
+        <f t="shared" si="21"/>
+        <v>19446.489368983679</v>
+      </c>
+      <c r="E138" s="129">
+        <f t="shared" si="24"/>
+        <v>369.98647962297719</v>
+      </c>
+      <c r="F138" s="93">
         <f t="shared" si="20"/>
-        <v>24274.702601296562</v>
-      </c>
-      <c r="E138" s="129">
-        <f t="shared" si="23"/>
-        <v>461.84746197291787</v>
-      </c>
-      <c r="F138" s="93">
-        <f t="shared" si="19"/>
-        <v>1620.517410431291</v>
+        <v>1298.1981741157094</v>
       </c>
     </row>
     <row r="139" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="108">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B139" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A139)*recentSyncTime15/365</f>
-        <v>17601.996660232544</v>
+        <f t="shared" si="19"/>
+        <v>14081.597328186035</v>
       </c>
       <c r="C139" s="104">
-        <f t="shared" si="22"/>
-        <v>172.9951171875</v>
+        <f t="shared" si="23"/>
+        <v>115.330078125</v>
       </c>
       <c r="D139" s="114">
+        <f t="shared" si="21"/>
+        <v>24274.702601296562</v>
+      </c>
+      <c r="E139" s="129">
+        <f t="shared" si="24"/>
+        <v>461.84746197291787</v>
+      </c>
+      <c r="F139" s="93">
         <f t="shared" si="20"/>
-        <v>30293.26458672115</v>
-      </c>
-      <c r="E139" s="129">
-        <f t="shared" si="23"/>
-        <v>576.35587113244208</v>
-      </c>
-      <c r="F139" s="93">
-        <f t="shared" si="19"/>
-        <v>2022.3013022190946</v>
+        <v>1620.517410431291</v>
       </c>
     </row>
     <row r="140" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="108">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B140" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A140)*recentSyncTime15/365</f>
-        <v>22002.49582529068</v>
+        <f t="shared" si="19"/>
+        <v>17601.996660232544</v>
       </c>
       <c r="C140" s="104">
-        <f t="shared" si="22"/>
-        <v>259.49267578125</v>
+        <f t="shared" si="23"/>
+        <v>172.9951171875</v>
       </c>
       <c r="D140" s="114">
+        <f t="shared" si="21"/>
+        <v>30293.26458672115</v>
+      </c>
+      <c r="E140" s="129">
+        <f t="shared" si="24"/>
+        <v>576.35587113244208</v>
+      </c>
+      <c r="F140" s="93">
         <f t="shared" si="20"/>
-        <v>37791.410236052106</v>
-      </c>
-      <c r="E140" s="129">
-        <f t="shared" si="23"/>
-        <v>719.01465441499442</v>
-      </c>
-      <c r="F140" s="93">
-        <f t="shared" si="19"/>
-        <v>2522.8584365438401</v>
+        <v>2022.3013022190946</v>
       </c>
     </row>
     <row r="141" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="108">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B141" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A141)*recentSyncTime15/365</f>
-        <v>27503.11978161335</v>
+        <f t="shared" si="19"/>
+        <v>22002.49582529068</v>
       </c>
       <c r="C141" s="104">
-        <f t="shared" si="22"/>
-        <v>364.61267578125</v>
+        <f t="shared" si="23"/>
+        <v>259.49267578125</v>
       </c>
       <c r="D141" s="114">
+        <f t="shared" si="21"/>
+        <v>37791.410236052106</v>
+      </c>
+      <c r="E141" s="129">
+        <f t="shared" si="24"/>
+        <v>719.01465441499442</v>
+      </c>
+      <c r="F141" s="93">
         <f t="shared" si="20"/>
-        <v>47169.309969660557</v>
-      </c>
-      <c r="E141" s="129">
-        <f t="shared" si="23"/>
-        <v>897.43740429338959</v>
-      </c>
-      <c r="F141" s="93">
-        <f t="shared" si="19"/>
-        <v>3148.9031729592621</v>
+        <v>2522.8584365438401</v>
       </c>
     </row>
     <row r="142" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="108">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B142" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A142)*recentSyncTime15/365</f>
-        <v>34378.899727016687</v>
+        <f t="shared" si="19"/>
+        <v>27503.11978161335</v>
       </c>
       <c r="C142" s="104">
-        <f t="shared" si="22"/>
-        <v>469.73267578125001</v>
+        <f t="shared" si="23"/>
+        <v>364.61267578125</v>
       </c>
       <c r="D142" s="114">
+        <f t="shared" si="21"/>
+        <v>47169.309969660557</v>
+      </c>
+      <c r="E142" s="129">
+        <f t="shared" si="24"/>
+        <v>897.43740429338959</v>
+      </c>
+      <c r="F142" s="93">
         <f t="shared" si="20"/>
-        <v>58937.36177952827</v>
-      </c>
-      <c r="E142" s="129">
-        <f t="shared" si="23"/>
-        <v>1121.3348892604313</v>
-      </c>
-      <c r="F142" s="93">
-        <f t="shared" si="19"/>
-        <v>3934.5083833699346</v>
+        <v>3148.9031729592621</v>
       </c>
     </row>
     <row r="143" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="108">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B143" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A143)*recentSyncTime15/365</f>
-        <v>42973.624658770859</v>
+        <f t="shared" si="19"/>
+        <v>34378.899727016687</v>
       </c>
       <c r="C143" s="104">
-        <f t="shared" si="22"/>
-        <v>574.85267578125001</v>
+        <f t="shared" si="23"/>
+        <v>469.73267578125001</v>
       </c>
       <c r="D143" s="114">
+        <f t="shared" si="21"/>
+        <v>58937.36177952827</v>
+      </c>
+      <c r="E143" s="129">
+        <f t="shared" si="24"/>
+        <v>1121.3348892604313</v>
+      </c>
+      <c r="F143" s="93">
         <f t="shared" si="20"/>
-        <v>73693.103684720045</v>
-      </c>
-      <c r="E143" s="129">
-        <f t="shared" si="23"/>
-        <v>1402.075793088281</v>
-      </c>
-      <c r="F143" s="93">
-        <f t="shared" si="19"/>
-        <v>4919.5641862746706</v>
+        <v>3934.5083833699346</v>
       </c>
     </row>
     <row r="144" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="108">
+        <v>14</v>
+      </c>
+      <c r="B144" s="130">
+        <f t="shared" si="19"/>
+        <v>42973.624658770859</v>
+      </c>
+      <c r="C144" s="104">
+        <f t="shared" si="23"/>
+        <v>574.85267578125001</v>
+      </c>
+      <c r="D144" s="114">
+        <f t="shared" si="21"/>
+        <v>73693.103684720045</v>
+      </c>
+      <c r="E144" s="129">
+        <f t="shared" si="24"/>
+        <v>1402.075793088281</v>
+      </c>
+      <c r="F144" s="93">
+        <f t="shared" si="20"/>
+        <v>4919.5641862746706</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="108">
         <v>15</v>
       </c>
-      <c r="B144" s="130">
-        <f>bandwidth15*syncResourcePercentage15*mbToGB*secondsPerYear*POWER(1+bandwidthGrowth,A144)*recentSyncTime15/365</f>
+      <c r="B145" s="130">
+        <f t="shared" si="19"/>
         <v>53717.030823463567</v>
       </c>
-      <c r="C144" s="104">
-        <f t="shared" si="22"/>
+      <c r="C145" s="104">
+        <f t="shared" si="23"/>
         <v>679.97267578125002</v>
       </c>
-      <c r="D144" s="114">
+      <c r="D145" s="114">
+        <f t="shared" si="21"/>
+        <v>92183.458209066885</v>
+      </c>
+      <c r="E145" s="129">
+        <f t="shared" si="24"/>
+        <v>1753.87097049214</v>
+      </c>
+      <c r="F145" s="93">
         <f t="shared" si="20"/>
-        <v>92183.458209066885</v>
-      </c>
-      <c r="E144" s="129">
-        <f t="shared" si="23"/>
-        <v>1753.87097049214</v>
-      </c>
-      <c r="F144" s="93">
-        <f t="shared" si="19"/>
         <v>6153.9332297969822</v>
       </c>
     </row>
-    <row r="145" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="113" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="109" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="113" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" s="108" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B149" s="109" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B150" s="109" t="s">
+        <v>111</v>
+      </c>
+      <c r="C150" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="D150" s="109" t="s">
+        <v>32</v>
+      </c>
+      <c r="E150" s="109" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="C149" s="109" t="s">
+      <c r="C151" s="109" t="s">
         <v>107</v>
       </c>
-      <c r="D149" s="109" t="s">
-        <v>32</v>
-      </c>
-      <c r="E149" s="109" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="138" t="s">
+      <c r="D151" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="E151" s="109" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="108">
+        <v>0</v>
+      </c>
+      <c r="B152">
+        <f t="shared" ref="B152:B167" si="25">FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A152)*ongoingResourcePercentage15, 2),1)</f>
+        <v>29</v>
+      </c>
+      <c r="C152" s="141">
+        <f t="shared" ref="C152:C167" si="26">$B$125*32*(LOG((endGameUsers*1000*1000*1000)*utxosPerUserEndGame, 2)-B152)</f>
+        <v>674.63737880070312</v>
+      </c>
+      <c r="D152" s="129">
+        <f t="shared" ref="D152:D167" si="27">(bandwidth15*ongoingResourcePercentage15*POWER(1+bandwidthGrowth,A152)*mbToGB*1000)*secondsPerBlock/2</f>
+        <v>187.5</v>
+      </c>
+      <c r="E152" s="111">
+        <f t="shared" ref="E152:E167" si="28">D152*1000*1000/secondsPerBlock/(2*(endGameTransactionSize+C152))</f>
+        <v>135.91242150024675</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="108">
+        <v>1</v>
+      </c>
+      <c r="B153" s="108">
+        <f t="shared" si="25"/>
+        <v>29</v>
+      </c>
+      <c r="C153" s="141">
+        <f t="shared" si="26"/>
+        <v>674.63737880070312</v>
+      </c>
+      <c r="D153" s="129">
+        <f t="shared" si="27"/>
+        <v>234.375</v>
+      </c>
+      <c r="E153" s="111">
+        <f t="shared" si="28"/>
+        <v>169.89052687530844</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="108">
+        <v>2</v>
+      </c>
+      <c r="B154" s="108">
+        <f t="shared" si="25"/>
+        <v>29</v>
+      </c>
+      <c r="C154" s="141">
+        <f t="shared" si="26"/>
+        <v>674.63737880070312</v>
+      </c>
+      <c r="D154" s="129">
+        <f t="shared" si="27"/>
+        <v>292.96875</v>
+      </c>
+      <c r="E154" s="111">
+        <f t="shared" si="28"/>
+        <v>212.36315859413554</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="108">
+        <v>3</v>
+      </c>
+      <c r="B155" s="108">
+        <f t="shared" si="25"/>
+        <v>30</v>
+      </c>
+      <c r="C155" s="141">
+        <f t="shared" si="26"/>
+        <v>610.63737880070312</v>
+      </c>
+      <c r="D155" s="129">
+        <f t="shared" si="27"/>
+        <v>366.2109375</v>
+      </c>
+      <c r="E155" s="111">
+        <f t="shared" si="28"/>
+        <v>281.10286842474585</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="108">
+        <v>4</v>
+      </c>
+      <c r="B156" s="108">
+        <f t="shared" si="25"/>
+        <v>30</v>
+      </c>
+      <c r="C156" s="141">
+        <f t="shared" si="26"/>
+        <v>610.63737880070312</v>
+      </c>
+      <c r="D156" s="129">
+        <f t="shared" si="27"/>
+        <v>457.763671875</v>
+      </c>
+      <c r="E156" s="111">
+        <f t="shared" si="28"/>
+        <v>351.3785855309323</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="108">
+        <v>5</v>
+      </c>
+      <c r="B157" s="108">
+        <f t="shared" si="25"/>
+        <v>30</v>
+      </c>
+      <c r="C157" s="141">
+        <f t="shared" si="26"/>
+        <v>610.63737880070312</v>
+      </c>
+      <c r="D157" s="129">
+        <f t="shared" si="27"/>
+        <v>572.20458984375</v>
+      </c>
+      <c r="E157" s="111">
+        <f t="shared" si="28"/>
+        <v>439.22323191366536</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="108">
+        <v>6</v>
+      </c>
+      <c r="B158" s="108">
+        <f t="shared" si="25"/>
+        <v>30</v>
+      </c>
+      <c r="C158" s="141">
+        <f t="shared" si="26"/>
+        <v>610.63737880070312</v>
+      </c>
+      <c r="D158" s="129">
+        <f t="shared" si="27"/>
+        <v>715.2557373046875</v>
+      </c>
+      <c r="E158" s="111">
+        <f t="shared" si="28"/>
+        <v>549.02903989208176</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="108">
+        <v>7</v>
+      </c>
+      <c r="B159" s="108">
+        <f t="shared" si="25"/>
+        <v>30</v>
+      </c>
+      <c r="C159" s="141">
+        <f t="shared" si="26"/>
+        <v>610.63737880070312</v>
+      </c>
+      <c r="D159" s="129">
+        <f t="shared" si="27"/>
+        <v>894.06967163085937</v>
+      </c>
+      <c r="E159" s="111">
+        <f t="shared" si="28"/>
+        <v>686.28629986510214</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="108">
         <v>8</v>
       </c>
-      <c r="B150" s="109" t="s">
-        <v>113</v>
-      </c>
-      <c r="C150" s="109" t="s">
-        <v>108</v>
-      </c>
-      <c r="D150" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="E150" s="109" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="108">
-        <v>0</v>
-      </c>
-      <c r="B151">
-        <f t="shared" ref="B151:B166" si="24">FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A151)*ongoingResourcePercentage15, 2),1)</f>
-        <v>29</v>
-      </c>
-      <c r="C151" s="141">
-        <f t="shared" ref="C151:C166" si="25">$B$124*32*(LOG((endGameUsers*1000*1000*1000)*utxosPerUserEndGame, 2)-B151)</f>
-        <v>674.63737880070312</v>
-      </c>
-      <c r="D151" s="129">
-        <f t="shared" ref="D151:D166" si="26">(bandwidth15*ongoingResourcePercentage15*POWER(1+bandwidthGrowth,A151)*mbToGB*1000)*secondsPerBlock/2</f>
-        <v>187.5</v>
-      </c>
-      <c r="E151" s="111">
-        <f t="shared" ref="E151:E166" si="27">D151*1000*1000/secondsPerBlock/(2*(endGameTransactionSize+C151))</f>
-        <v>135.91242150024675</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="108">
-        <v>1</v>
-      </c>
-      <c r="B152" s="108">
-        <f t="shared" si="24"/>
-        <v>29</v>
-      </c>
-      <c r="C152" s="141">
+      <c r="B160" s="108">
         <f t="shared" si="25"/>
-        <v>674.63737880070312</v>
-      </c>
-      <c r="D152" s="129">
+        <v>31</v>
+      </c>
+      <c r="C160" s="141">
         <f t="shared" si="26"/>
-        <v>234.375</v>
-      </c>
-      <c r="E152" s="111">
+        <v>546.63737880070312</v>
+      </c>
+      <c r="D160" s="129">
         <f t="shared" si="27"/>
-        <v>169.89052687530844</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="108">
-        <v>2</v>
-      </c>
-      <c r="B153" s="108">
-        <f t="shared" si="24"/>
-        <v>29</v>
-      </c>
-      <c r="C153" s="141">
-        <f t="shared" si="25"/>
-        <v>674.63737880070312</v>
-      </c>
-      <c r="D153" s="129">
-        <f t="shared" si="26"/>
-        <v>292.96875</v>
-      </c>
-      <c r="E153" s="111">
-        <f t="shared" si="27"/>
-        <v>212.36315859413554</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="108">
-        <v>3</v>
-      </c>
-      <c r="B154" s="108">
-        <f t="shared" si="24"/>
-        <v>30</v>
-      </c>
-      <c r="C154" s="141">
-        <f t="shared" si="25"/>
-        <v>610.63737880070312</v>
-      </c>
-      <c r="D154" s="129">
-        <f t="shared" si="26"/>
-        <v>366.2109375</v>
-      </c>
-      <c r="E154" s="111">
-        <f t="shared" si="27"/>
-        <v>281.10286842474585</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="108">
-        <v>4</v>
-      </c>
-      <c r="B155" s="108">
-        <f t="shared" si="24"/>
-        <v>30</v>
-      </c>
-      <c r="C155" s="141">
-        <f t="shared" si="25"/>
-        <v>610.63737880070312</v>
-      </c>
-      <c r="D155" s="129">
-        <f t="shared" si="26"/>
-        <v>457.763671875</v>
-      </c>
-      <c r="E155" s="111">
-        <f t="shared" si="27"/>
-        <v>351.3785855309323</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="108">
-        <v>5</v>
-      </c>
-      <c r="B156" s="108">
-        <f t="shared" si="24"/>
-        <v>30</v>
-      </c>
-      <c r="C156" s="141">
-        <f t="shared" si="25"/>
-        <v>610.63737880070312</v>
-      </c>
-      <c r="D156" s="129">
-        <f t="shared" si="26"/>
-        <v>572.20458984375</v>
-      </c>
-      <c r="E156" s="111">
-        <f t="shared" si="27"/>
-        <v>439.22323191366536</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" s="108">
-        <v>6</v>
-      </c>
-      <c r="B157" s="108">
-        <f t="shared" si="24"/>
-        <v>30</v>
-      </c>
-      <c r="C157" s="141">
-        <f t="shared" si="25"/>
-        <v>610.63737880070312</v>
-      </c>
-      <c r="D157" s="129">
-        <f t="shared" si="26"/>
-        <v>715.2557373046875</v>
-      </c>
-      <c r="E157" s="111">
-        <f t="shared" si="27"/>
-        <v>549.02903989208176</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="108">
-        <v>7</v>
-      </c>
-      <c r="B158" s="108">
-        <f t="shared" si="24"/>
-        <v>30</v>
-      </c>
-      <c r="C158" s="141">
-        <f t="shared" si="25"/>
-        <v>610.63737880070312</v>
-      </c>
-      <c r="D158" s="129">
-        <f t="shared" si="26"/>
-        <v>894.06967163085937</v>
-      </c>
-      <c r="E158" s="111">
-        <f t="shared" si="27"/>
-        <v>686.28629986510214</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="108">
-        <v>8</v>
-      </c>
-      <c r="B159" s="108">
-        <f t="shared" si="24"/>
-        <v>31</v>
-      </c>
-      <c r="C159" s="141">
-        <f t="shared" si="25"/>
-        <v>546.63737880070312</v>
-      </c>
-      <c r="D159" s="129">
-        <f t="shared" si="26"/>
         <v>1117.5870895385742</v>
       </c>
-      <c r="E159" s="111">
-        <f t="shared" si="27"/>
+      <c r="E160" s="111">
+        <f t="shared" si="28"/>
         <v>911.59798372760713</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="108">
-        <v>9</v>
-      </c>
-      <c r="B160" s="108">
-        <f t="shared" si="24"/>
-        <v>31</v>
-      </c>
-      <c r="C160" s="141">
-        <f t="shared" si="25"/>
-        <v>546.63737880070312</v>
-      </c>
-      <c r="D160" s="129">
-        <f t="shared" si="26"/>
-        <v>1396.9838619232178</v>
-      </c>
-      <c r="E160" s="111">
-        <f t="shared" si="27"/>
-        <v>1139.4974796595088</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="108">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B161" s="108">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>31</v>
       </c>
       <c r="C161" s="141">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>546.63737880070312</v>
       </c>
       <c r="D161" s="129">
-        <f t="shared" si="26"/>
-        <v>1746.2298274040222</v>
+        <f t="shared" si="27"/>
+        <v>1396.9838619232178</v>
       </c>
       <c r="E161" s="111">
-        <f t="shared" si="27"/>
-        <v>1424.371849574386</v>
+        <f t="shared" si="28"/>
+        <v>1139.4974796595088</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="108">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B162" s="108">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>31</v>
       </c>
       <c r="C162" s="141">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>546.63737880070312</v>
       </c>
       <c r="D162" s="129">
-        <f t="shared" si="26"/>
-        <v>2182.7872842550278</v>
+        <f t="shared" si="27"/>
+        <v>1746.2298274040222</v>
       </c>
       <c r="E162" s="111">
-        <f t="shared" si="27"/>
-        <v>1780.4648119679825</v>
+        <f t="shared" si="28"/>
+        <v>1424.371849574386</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="108">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B163" s="108">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>31</v>
       </c>
       <c r="C163" s="141">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>546.63737880070312</v>
       </c>
       <c r="D163" s="129">
-        <f t="shared" si="26"/>
-        <v>2728.4841053187847</v>
+        <f t="shared" si="27"/>
+        <v>2182.7872842550278</v>
       </c>
       <c r="E163" s="111">
-        <f t="shared" si="27"/>
-        <v>2225.5810149599783</v>
+        <f t="shared" si="28"/>
+        <v>1780.4648119679825</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="108">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B164" s="108">
-        <f t="shared" si="24"/>
-        <v>32</v>
+        <f t="shared" si="25"/>
+        <v>31</v>
       </c>
       <c r="C164" s="141">
-        <f t="shared" si="25"/>
-        <v>482.63737880070312</v>
+        <f t="shared" si="26"/>
+        <v>546.63737880070312</v>
       </c>
       <c r="D164" s="129">
-        <f t="shared" si="26"/>
-        <v>3410.6051316484809</v>
+        <f t="shared" si="27"/>
+        <v>2728.4841053187847</v>
       </c>
       <c r="E164" s="111">
-        <f t="shared" si="27"/>
-        <v>2967.8989207791706</v>
+        <f t="shared" si="28"/>
+        <v>2225.5810149599783</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="108">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B165" s="108">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>32</v>
       </c>
       <c r="C165" s="141">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>482.63737880070312</v>
       </c>
       <c r="D165" s="129">
-        <f t="shared" si="26"/>
-        <v>4263.2564145606011</v>
+        <f t="shared" si="27"/>
+        <v>3410.6051316484809</v>
       </c>
       <c r="E165" s="111">
-        <f t="shared" si="27"/>
-        <v>3709.8736509739633</v>
+        <f t="shared" si="28"/>
+        <v>2967.8989207791706</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="108">
+        <v>14</v>
+      </c>
+      <c r="B166" s="108">
+        <f t="shared" si="25"/>
+        <v>32</v>
+      </c>
+      <c r="C166" s="141">
+        <f t="shared" si="26"/>
+        <v>482.63737880070312</v>
+      </c>
+      <c r="D166" s="129">
+        <f t="shared" si="27"/>
+        <v>4263.2564145606011</v>
+      </c>
+      <c r="E166" s="111">
+        <f t="shared" si="28"/>
+        <v>3709.8736509739633</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="108">
         <v>15</v>
       </c>
-      <c r="B166" s="108">
-        <f t="shared" si="24"/>
+      <c r="B167" s="108">
+        <f t="shared" si="25"/>
         <v>32</v>
       </c>
-      <c r="C166" s="141">
-        <f t="shared" si="25"/>
+      <c r="C167" s="141">
+        <f t="shared" si="26"/>
         <v>482.63737880070312</v>
       </c>
-      <c r="D166" s="129">
-        <f t="shared" si="26"/>
+      <c r="D167" s="129">
+        <f t="shared" si="27"/>
         <v>5329.0705182007514</v>
       </c>
-      <c r="E166" s="111">
-        <f t="shared" si="27"/>
+      <c r="E167" s="111">
+        <f t="shared" si="28"/>
         <v>4637.342063717454</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="113" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="108"/>
-      <c r="B170" s="109" t="s">
-        <v>114</v>
-      </c>
-      <c r="C170" s="108"/>
-      <c r="D170" s="108"/>
-      <c r="E170" s="108"/>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="113" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="108"/>
       <c r="B171" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="C171" s="108"/>
+      <c r="D171" s="108"/>
+      <c r="E171" s="108"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="108"/>
+      <c r="B172" s="109" t="s">
+        <v>111</v>
+      </c>
+      <c r="C172" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="D172" s="109" t="s">
+        <v>32</v>
+      </c>
+      <c r="E172" s="109" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="139" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="C171" s="109" t="s">
+      <c r="C173" s="109" t="s">
         <v>107</v>
       </c>
-      <c r="D171" s="109" t="s">
-        <v>32</v>
-      </c>
-      <c r="E171" s="109" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="139" t="s">
-        <v>8</v>
-      </c>
-      <c r="B172" s="109" t="s">
-        <v>113</v>
-      </c>
-      <c r="C172" s="109" t="s">
-        <v>108</v>
-      </c>
-      <c r="D172" s="109" t="s">
+      <c r="D173" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="E172" s="109" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="108">
-        <v>0</v>
-      </c>
-      <c r="B173" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A173)*ongoingResourcePercentage15, 2),1)</f>
-        <v>29</v>
-      </c>
-      <c r="C173" s="141">
-        <f t="shared" ref="C173:C188" si="28">$B$124*32*(LOG((endGameUsers*1000*1000*1000)*utxosPerUserEndGame, 2)-B173)</f>
-        <v>674.63737880070312</v>
-      </c>
-      <c r="D173" s="129">
-        <f t="shared" ref="D173:D188" si="29">(bandwidth15*endGameEmergencyUsage*POWER(1+bandwidthGrowth,A173)*mbToGB*1000)*secondsPerBlock/2</f>
-        <v>1406.25</v>
-      </c>
-      <c r="E173" s="111">
-        <f t="shared" ref="E173:E188" si="30">D173*1000*1000/secondsPerBlock/(2*(endGameTransactionSize+C173))</f>
-        <v>1019.3431612518506</v>
+      <c r="E173" s="109" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B174" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A174)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" ref="B174:B189" si="29">FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A174)*ongoingResourcePercentage15, 2),1)</f>
         <v>29</v>
       </c>
       <c r="C174" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="C174:C189" si="30">$B$125*32*(LOG((endGameUsers*1000*1000*1000)*utxosPerUserEndGame, 2)-B174)</f>
         <v>674.63737880070312</v>
       </c>
       <c r="D174" s="129">
-        <f t="shared" si="29"/>
-        <v>1757.8125</v>
+        <f t="shared" ref="D174:D189" si="31">(bandwidth15*endGameEmergencyUsage*POWER(1+bandwidthGrowth,A174)*mbToGB*1000)*secondsPerBlock/2</f>
+        <v>1406.25</v>
       </c>
       <c r="E174" s="111">
-        <f t="shared" si="30"/>
-        <v>1274.1789515648134</v>
+        <f t="shared" ref="E174:E189" si="32">D174*1000*1000/secondsPerBlock/(2*(endGameTransactionSize+C174))</f>
+        <v>1019.3431612518506</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B175" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A175)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>29</v>
       </c>
       <c r="C175" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>674.63737880070312</v>
       </c>
       <c r="D175" s="129">
-        <f t="shared" si="29"/>
-        <v>2197.265625</v>
+        <f t="shared" si="31"/>
+        <v>1757.8125</v>
       </c>
       <c r="E175" s="111">
-        <f t="shared" si="30"/>
-        <v>1592.7236894560167</v>
+        <f t="shared" si="32"/>
+        <v>1274.1789515648134</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="108">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B176" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A176)*ongoingResourcePercentage15, 2),1)</f>
-        <v>30</v>
+        <f t="shared" si="29"/>
+        <v>29</v>
       </c>
       <c r="C176" s="141">
-        <f t="shared" si="28"/>
-        <v>610.63737880070312</v>
+        <f t="shared" si="30"/>
+        <v>674.63737880070312</v>
       </c>
       <c r="D176" s="129">
-        <f t="shared" si="29"/>
-        <v>2746.58203125</v>
+        <f t="shared" si="31"/>
+        <v>2197.265625</v>
       </c>
       <c r="E176" s="111">
-        <f t="shared" si="30"/>
-        <v>2108.2715131855939</v>
+        <f t="shared" si="32"/>
+        <v>1592.7236894560167</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B177" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A177)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>30</v>
       </c>
       <c r="C177" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>610.63737880070312</v>
       </c>
       <c r="D177" s="129">
-        <f t="shared" si="29"/>
-        <v>3433.2275390625</v>
+        <f t="shared" si="31"/>
+        <v>2746.58203125</v>
       </c>
       <c r="E177" s="111">
-        <f t="shared" si="30"/>
-        <v>2635.3393914819922</v>
+        <f t="shared" si="32"/>
+        <v>2108.2715131855939</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="108">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B178" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A178)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>30</v>
       </c>
       <c r="C178" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>610.63737880070312</v>
       </c>
       <c r="D178" s="129">
-        <f t="shared" si="29"/>
-        <v>4291.534423828125</v>
+        <f t="shared" si="31"/>
+        <v>3433.2275390625</v>
       </c>
       <c r="E178" s="111">
-        <f t="shared" si="30"/>
-        <v>3294.1742393524901</v>
+        <f t="shared" si="32"/>
+        <v>2635.3393914819922</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="108">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B179" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A179)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>30</v>
       </c>
       <c r="C179" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>610.63737880070312</v>
       </c>
       <c r="D179" s="129">
-        <f t="shared" si="29"/>
-        <v>5364.4180297851562</v>
+        <f t="shared" si="31"/>
+        <v>4291.534423828125</v>
       </c>
       <c r="E179" s="111">
-        <f t="shared" si="30"/>
-        <v>4117.7177991906128</v>
+        <f t="shared" si="32"/>
+        <v>3294.1742393524901</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="108">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B180" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A180)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>30</v>
       </c>
       <c r="C180" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>610.63737880070312</v>
       </c>
       <c r="D180" s="129">
-        <f t="shared" si="29"/>
-        <v>6705.5225372314453</v>
+        <f t="shared" si="31"/>
+        <v>5364.4180297851562</v>
       </c>
       <c r="E180" s="111">
-        <f t="shared" si="30"/>
-        <v>5147.1472489882663</v>
+        <f t="shared" si="32"/>
+        <v>4117.7177991906128</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="108">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B181" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A181)*ongoingResourcePercentage15, 2),1)</f>
-        <v>31</v>
+        <f t="shared" si="29"/>
+        <v>30</v>
       </c>
       <c r="C181" s="141">
-        <f t="shared" si="28"/>
-        <v>546.63737880070312</v>
+        <f t="shared" si="30"/>
+        <v>610.63737880070312</v>
       </c>
       <c r="D181" s="129">
-        <f t="shared" si="29"/>
-        <v>8381.9031715393066</v>
+        <f t="shared" si="31"/>
+        <v>6705.5225372314453</v>
       </c>
       <c r="E181" s="111">
-        <f t="shared" si="30"/>
-        <v>6836.984877957053</v>
+        <f t="shared" si="32"/>
+        <v>5147.1472489882663</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="108">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B182" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A182)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>31</v>
       </c>
       <c r="C182" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>546.63737880070312</v>
       </c>
       <c r="D182" s="129">
-        <f t="shared" si="29"/>
-        <v>10477.378964424133</v>
+        <f t="shared" si="31"/>
+        <v>8381.9031715393066</v>
       </c>
       <c r="E182" s="111">
-        <f t="shared" si="30"/>
-        <v>8546.2310974463162</v>
+        <f t="shared" si="32"/>
+        <v>6836.984877957053</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="108">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B183" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A183)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>31</v>
       </c>
       <c r="C183" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>546.63737880070312</v>
       </c>
       <c r="D183" s="129">
-        <f t="shared" si="29"/>
-        <v>13096.723705530167</v>
+        <f t="shared" si="31"/>
+        <v>10477.378964424133</v>
       </c>
       <c r="E183" s="111">
-        <f t="shared" si="30"/>
-        <v>10682.788871807896</v>
+        <f t="shared" si="32"/>
+        <v>8546.2310974463162</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="108">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B184" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A184)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>31</v>
       </c>
       <c r="C184" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>546.63737880070312</v>
       </c>
       <c r="D184" s="129">
-        <f t="shared" si="29"/>
-        <v>16370.904631912708</v>
+        <f t="shared" si="31"/>
+        <v>13096.723705530167</v>
       </c>
       <c r="E184" s="111">
-        <f t="shared" si="30"/>
-        <v>13353.48608975987</v>
+        <f t="shared" si="32"/>
+        <v>10682.788871807896</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="108">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B185" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A185)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>31</v>
       </c>
       <c r="C185" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>546.63737880070312</v>
       </c>
       <c r="D185" s="129">
-        <f t="shared" si="29"/>
-        <v>20463.630789890885</v>
+        <f t="shared" si="31"/>
+        <v>16370.904631912708</v>
       </c>
       <c r="E185" s="111">
-        <f t="shared" si="30"/>
-        <v>16691.857612199838</v>
+        <f t="shared" si="32"/>
+        <v>13353.48608975987</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="108">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B186" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A186)*ongoingResourcePercentage15, 2),1)</f>
-        <v>32</v>
+        <f t="shared" si="29"/>
+        <v>31</v>
       </c>
       <c r="C186" s="141">
-        <f t="shared" si="28"/>
-        <v>482.63737880070312</v>
+        <f t="shared" si="30"/>
+        <v>546.63737880070312</v>
       </c>
       <c r="D186" s="129">
-        <f t="shared" si="29"/>
-        <v>25579.538487363607</v>
+        <f t="shared" si="31"/>
+        <v>20463.630789890885</v>
       </c>
       <c r="E186" s="111">
-        <f t="shared" si="30"/>
-        <v>22259.241905843781</v>
+        <f t="shared" si="32"/>
+        <v>16691.857612199838</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="108">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B187" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A187)*ongoingResourcePercentage15, 2),1)</f>
+        <f t="shared" si="29"/>
         <v>32</v>
       </c>
       <c r="C187" s="141">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>482.63737880070312</v>
       </c>
       <c r="D187" s="129">
-        <f t="shared" si="29"/>
-        <v>31974.423109204508</v>
+        <f t="shared" si="31"/>
+        <v>25579.538487363607</v>
       </c>
       <c r="E187" s="111">
-        <f t="shared" si="30"/>
-        <v>27824.052382304726</v>
+        <f t="shared" si="32"/>
+        <v>22259.241905843781</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="108">
+        <v>14</v>
+      </c>
+      <c r="B188" s="108">
+        <f t="shared" si="29"/>
+        <v>32</v>
+      </c>
+      <c r="C188" s="141">
+        <f t="shared" si="30"/>
+        <v>482.63737880070312</v>
+      </c>
+      <c r="D188" s="129">
+        <f t="shared" si="31"/>
+        <v>31974.423109204508</v>
+      </c>
+      <c r="E188" s="111">
+        <f t="shared" si="32"/>
+        <v>27824.052382304726</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="108">
         <v>15</v>
       </c>
-      <c r="B188" s="108">
-        <f>FLOOR(LOG((memory15*1000*1000*1000)*POWER(1+memoryGrowth,A188)*ongoingResourcePercentage15, 2),1)</f>
+      <c r="B189" s="108">
+        <f t="shared" si="29"/>
         <v>32</v>
       </c>
-      <c r="C188" s="141">
-        <f t="shared" si="28"/>
+      <c r="C189" s="141">
+        <f t="shared" si="30"/>
         <v>482.63737880070312</v>
       </c>
-      <c r="D188" s="129">
-        <f t="shared" si="29"/>
+      <c r="D189" s="129">
+        <f t="shared" si="31"/>
         <v>39968.028886505635</v>
       </c>
-      <c r="E188" s="111">
-        <f t="shared" si="30"/>
+      <c r="E189" s="111">
+        <f t="shared" si="32"/>
         <v>34780.065477880904</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="113" t="s">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="113" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B193" s="109" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B192" s="109" t="s">
+      <c r="C193" s="109" t="s">
         <v>126</v>
       </c>
-      <c r="C192" s="109" t="s">
+      <c r="D193" s="109" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B194" s="109" t="s">
+        <v>110</v>
+      </c>
+      <c r="C194" s="109" t="s">
         <v>127</v>
       </c>
-      <c r="D192" s="109" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="109" t="s">
-        <v>111</v>
-      </c>
-      <c r="C193" s="109" t="s">
-        <v>128</v>
-      </c>
-      <c r="D193" s="109" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="121">
+      <c r="D194" s="109" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B195" s="121">
         <v>3</v>
       </c>
-      <c r="C194" s="24">
+      <c r="C195" s="24">
         <v>30</v>
       </c>
-      <c r="D194" s="144">
-        <f>(endGameUsers*1000*1000*1000)*(B194/2)/(C194*24*60*60)</f>
+      <c r="D195" s="144">
+        <f>(endGameUsers*1000*1000*1000)*(B195/2)/(C195*24*60*60)</f>
         <v>4629.6296296296296</v>
       </c>
     </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" s="113" t="s">
+        <v>133</v>
+      </c>
+      <c r="D197" s="109"/>
+      <c r="E197" s="109"/>
+      <c r="F197" s="109"/>
+      <c r="G197" s="109" t="s">
+        <v>32</v>
+      </c>
+      <c r="H197" s="109" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D198" s="109" t="s">
+        <v>68</v>
+      </c>
+      <c r="E198" s="109" t="s">
+        <v>69</v>
+      </c>
+      <c r="F198" s="109" t="s">
+        <v>18</v>
+      </c>
+      <c r="G198" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="H198" s="109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A199" s="147" t="s">
+        <v>130</v>
+      </c>
+      <c r="B199" s="147"/>
+      <c r="C199" s="147"/>
+      <c r="D199" s="106" t="str">
+        <f>$A$120</f>
+        <v>10th %ile</v>
+      </c>
+      <c r="E199" s="111">
+        <f>E152</f>
+        <v>135.91242150024675</v>
+      </c>
+      <c r="F199" s="134">
+        <f>D152</f>
+        <v>187.5</v>
+      </c>
+      <c r="G199" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H199" s="135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A200" s="147" t="s">
+        <v>131</v>
+      </c>
+      <c r="B200" s="147"/>
+      <c r="C200" s="147"/>
+      <c r="D200" s="106" t="str">
+        <f>$A$120</f>
+        <v>10th %ile</v>
+      </c>
+      <c r="E200" s="46">
+        <f>F130</f>
+        <v>218.95015316067949</v>
+      </c>
+      <c r="F200" s="134">
+        <f>E130</f>
+        <v>62.400793650793652</v>
+      </c>
+      <c r="G200" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H200" s="135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A201" s="147" t="s">
+        <v>117</v>
+      </c>
+      <c r="B201" s="147"/>
+      <c r="C201" s="147"/>
+      <c r="D201" s="106" t="str">
+        <f>$A$120</f>
+        <v>10th %ile</v>
+      </c>
+      <c r="E201" s="111">
+        <f>E174</f>
+        <v>1019.3431612518506</v>
+      </c>
+      <c r="F201" s="134">
+        <f>D174</f>
+        <v>1406.25</v>
+      </c>
+      <c r="G201" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H201" s="135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="113" t="s">
+        <v>134</v>
+      </c>
+      <c r="B203" s="108"/>
+      <c r="C203" s="108"/>
+      <c r="D203" s="109"/>
+      <c r="E203" s="109"/>
+      <c r="F203" s="109"/>
+      <c r="G203" s="109" t="s">
+        <v>32</v>
+      </c>
+      <c r="H203" s="109" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="108"/>
+      <c r="B204" s="108"/>
+      <c r="C204" s="108"/>
+      <c r="D204" s="109" t="s">
+        <v>68</v>
+      </c>
+      <c r="E204" s="109" t="s">
+        <v>69</v>
+      </c>
+      <c r="F204" s="109" t="s">
+        <v>18</v>
+      </c>
+      <c r="G204" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="H204" s="109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A205" s="147" t="s">
+        <v>130</v>
+      </c>
+      <c r="B205" s="147"/>
+      <c r="C205" s="147"/>
+      <c r="D205" s="106" t="str">
+        <f>$A$120</f>
+        <v>10th %ile</v>
+      </c>
+      <c r="E205" s="111">
+        <f>E162</f>
+        <v>1424.371849574386</v>
+      </c>
+      <c r="F205" s="134">
+        <f>D162</f>
+        <v>1746.2298274040222</v>
+      </c>
+      <c r="G205" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H205" s="135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A206" s="147" t="s">
+        <v>131</v>
+      </c>
+      <c r="B206" s="147"/>
+      <c r="C206" s="147"/>
+      <c r="D206" s="106" t="str">
+        <f>$A$120</f>
+        <v>10th %ile</v>
+      </c>
+      <c r="E206" s="46">
+        <f>F140</f>
+        <v>2022.3013022190946</v>
+      </c>
+      <c r="F206" s="134">
+        <f>E140</f>
+        <v>576.35587113244208</v>
+      </c>
+      <c r="G206" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H206" s="135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A207" s="147" t="s">
+        <v>117</v>
+      </c>
+      <c r="B207" s="147"/>
+      <c r="C207" s="147"/>
+      <c r="D207" s="106" t="str">
+        <f>$A$120</f>
+        <v>10th %ile</v>
+      </c>
+      <c r="E207" s="111">
+        <f>E184</f>
+        <v>10682.788871807896</v>
+      </c>
+      <c r="F207" s="134">
+        <f>D184</f>
+        <v>13096.723705530167</v>
+      </c>
+      <c r="G207" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H207" s="135" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="A205:C205"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A207:C207"/>
+    <mergeCell ref="A199:C199"/>
+    <mergeCell ref="A200:C200"/>
+    <mergeCell ref="A201:C201"/>
     <mergeCell ref="A110:C110"/>
     <mergeCell ref="A111:C111"/>
     <mergeCell ref="A113:C113"/>
@@ -14746,7 +15048,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="lessThan" id="{CCBBA876-7DF4-468C-8839-EA8CEE01F71E}">
+          <x14:cfRule type="cellIs" priority="13" operator="lessThan" id="{CCBBA876-7DF4-468C-8839-EA8CEE01F71E}">
             <xm:f>'Current Bitcoin'!$C$19</xm:f>
             <x14:dxf>
               <font>
@@ -14762,7 +15064,7 @@
           <xm:sqref>F108:F109</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="lessThan" id="{A26EE87F-1C32-41E6-AC03-91370DB0C051}">
+          <x14:cfRule type="cellIs" priority="12" operator="lessThan" id="{A26EE87F-1C32-41E6-AC03-91370DB0C051}">
             <xm:f>'Current Bitcoin'!$C$19*1000/'Current Bitcoin'!$C$10/'Current Bitcoin'!$F$10</xm:f>
             <x14:dxf>
               <fill>
@@ -14772,10 +15074,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E108:E113</xm:sqref>
+          <xm:sqref>E108:E113 E201 E199</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="lessThan" id="{E16F959B-687E-48F0-9CC9-FF6B850AFA7F}">
+          <x14:cfRule type="cellIs" priority="11" operator="lessThan" id="{E16F959B-687E-48F0-9CC9-FF6B850AFA7F}">
             <xm:f>'Current Bitcoin'!$B$19</xm:f>
             <x14:dxf>
               <fill>
@@ -14788,7 +15090,7 @@
           <xm:sqref>G108:G110 G113</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{321EA6B3-025D-4AB3-8E5D-63B63B669534}">
+          <x14:cfRule type="cellIs" priority="6" operator="lessThan" id="{321EA6B3-025D-4AB3-8E5D-63B63B669534}">
             <xm:f>'Current Bitcoin'!$C$19/1000</xm:f>
             <x14:dxf>
               <font>
@@ -14802,6 +15104,51 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>F110:F113</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="lessThan" id="{8FB7B753-C1D7-4AB1-8C28-AF407E639D08}">
+            <xm:f>'Current Bitcoin'!$C$19/1000</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFBD1D7"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F199:F201</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="lessThan" id="{F69B60C6-2386-48E1-AF9E-DB8B0480E3DE}">
+            <xm:f>'Current Bitcoin'!$C$19*1000/'Current Bitcoin'!$C$10/'Current Bitcoin'!$F$10</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E207 E205</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{3D4FB6AB-EB61-4230-B3E1-02B34DEC6588}">
+            <xm:f>'Current Bitcoin'!$C$19/1000</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFBD1D7"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F205:F207</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
updating images an TOC
</commit_message>
<xml_diff>
--- a/bottlenecks.xlsx
+++ b/bottlenecks.xlsx
@@ -5883,7 +5883,7 @@
   <dimension ref="A1:L402"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14685,8 +14685,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C331" sqref="C331"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I313" sqref="I313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
minor information about 2014 era block propagation times
</commit_message>
<xml_diff>
--- a/bottlenecks.xlsx
+++ b/bottlenecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="15315" windowHeight="11880" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="2910" windowWidth="15315" windowHeight="11880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Current Bitcoin" sheetId="1" r:id="rId1"/>
@@ -1426,6 +1426,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="188" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1441,7 +1442,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1451,7 +1451,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBD1D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1466,16 +1476,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBD1D7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1537,17 +1537,13 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFB7B7"/>
+      <color rgb="FFF3C3C3"/>
+      <color rgb="FFEEA8A8"/>
       <color rgb="FFFF9F9F"/>
       <color rgb="FFFBD1D7"/>
     </mruColors>
@@ -1733,8 +1729,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="52568064"/>
-        <c:axId val="52732672"/>
+        <c:axId val="142776192"/>
+        <c:axId val="142778368"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1882,11 +1878,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="52978048"/>
-        <c:axId val="52734592"/>
+        <c:axId val="142781440"/>
+        <c:axId val="142779904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52568064"/>
+        <c:axId val="142776192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1915,7 +1911,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52732672"/>
+        <c:crossAx val="142778368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1923,7 +1919,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52732672"/>
+        <c:axId val="142778368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,12 +1944,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52568064"/>
+        <c:crossAx val="142776192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52734592"/>
+        <c:axId val="142779904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,12 +1975,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52978048"/>
+        <c:crossAx val="142781440"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="52978048"/>
+        <c:axId val="142781440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,7 +1990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52734592"/>
+        <c:crossAx val="142779904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2201,8 +2197,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="53009792"/>
-        <c:axId val="57104256"/>
+        <c:axId val="159011584"/>
+        <c:axId val="159013504"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2350,11 +2346,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70955008"/>
-        <c:axId val="57105792"/>
+        <c:axId val="159020928"/>
+        <c:axId val="159019392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53009792"/>
+        <c:axId val="159011584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2379,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57104256"/>
+        <c:crossAx val="159013504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2391,7 +2387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57104256"/>
+        <c:axId val="159013504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2416,12 +2412,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53009792"/>
+        <c:crossAx val="159011584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57105792"/>
+        <c:axId val="159019392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2447,12 +2443,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70955008"/>
+        <c:crossAx val="159020928"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="70955008"/>
+        <c:axId val="159020928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2462,7 +2458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57105792"/>
+        <c:crossAx val="159019392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2669,8 +2665,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="87526400"/>
-        <c:axId val="87536768"/>
+        <c:axId val="159047040"/>
+        <c:axId val="159053312"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2818,11 +2814,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88974848"/>
-        <c:axId val="87538304"/>
+        <c:axId val="159056640"/>
+        <c:axId val="159054848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87526400"/>
+        <c:axId val="159047040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2851,7 +2847,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87536768"/>
+        <c:crossAx val="159053312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2859,7 +2855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87536768"/>
+        <c:axId val="159053312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2884,12 +2880,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87526400"/>
+        <c:crossAx val="159047040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87538304"/>
+        <c:axId val="159054848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2915,12 +2911,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88974848"/>
+        <c:crossAx val="159056640"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="88974848"/>
+        <c:axId val="159056640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,7 +2926,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87538304"/>
+        <c:crossAx val="159054848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3138,8 +3134,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91772416"/>
-        <c:axId val="91813760"/>
+        <c:axId val="159087616"/>
+        <c:axId val="159093888"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3287,11 +3283,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92697728"/>
-        <c:axId val="91815296"/>
+        <c:axId val="159109504"/>
+        <c:axId val="159095424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91772416"/>
+        <c:axId val="159087616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3320,7 +3316,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91813760"/>
+        <c:crossAx val="159093888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3328,7 +3324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91813760"/>
+        <c:axId val="159093888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3353,12 +3349,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91772416"/>
+        <c:crossAx val="159087616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91815296"/>
+        <c:axId val="159095424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3384,12 +3380,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92697728"/>
+        <c:crossAx val="159109504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="92697728"/>
+        <c:axId val="159109504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3399,7 +3395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91815296"/>
+        <c:crossAx val="159095424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3754,11 +3750,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="50874240"/>
-        <c:axId val="50876416"/>
+        <c:axId val="159138944"/>
+        <c:axId val="159140864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50874240"/>
+        <c:axId val="159138944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3787,7 +3783,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50876416"/>
+        <c:crossAx val="159140864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3795,7 +3791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50876416"/>
+        <c:axId val="159140864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,7 +3816,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50874240"/>
+        <c:crossAx val="159138944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4025,8 +4021,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="50903296"/>
-        <c:axId val="50913664"/>
+        <c:axId val="159175808"/>
+        <c:axId val="159177728"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4174,11 +4170,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="50916736"/>
-        <c:axId val="50915200"/>
+        <c:axId val="159193344"/>
+        <c:axId val="159191808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50903296"/>
+        <c:axId val="159175808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4207,7 +4203,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50913664"/>
+        <c:crossAx val="159177728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4215,7 +4211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50913664"/>
+        <c:axId val="159177728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4240,12 +4236,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50903296"/>
+        <c:crossAx val="159175808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50915200"/>
+        <c:axId val="159191808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4271,12 +4267,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50916736"/>
+        <c:crossAx val="159193344"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="50916736"/>
+        <c:axId val="159193344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4286,7 +4282,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50915200"/>
+        <c:crossAx val="159191808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4640,11 +4636,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="51933184"/>
-        <c:axId val="51935104"/>
+        <c:axId val="159222400"/>
+        <c:axId val="159224576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51933184"/>
+        <c:axId val="159222400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4673,7 +4669,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51935104"/>
+        <c:crossAx val="159224576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4681,7 +4677,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51935104"/>
+        <c:axId val="159224576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4706,7 +4702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51933184"/>
+        <c:crossAx val="159222400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4911,11 +4907,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="52041600"/>
-        <c:axId val="52314112"/>
+        <c:axId val="142615680"/>
+        <c:axId val="142617600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52041600"/>
+        <c:axId val="142615680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4937,14 +4933,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52314112"/>
+        <c:crossAx val="142617600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4952,7 +4947,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52314112"/>
+        <c:axId val="142617600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4979,7 +4974,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52041600"/>
+        <c:crossAx val="142615680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5883,7 +5878,7 @@
   <dimension ref="A1:L402"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6081,20 +6076,20 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H7" s="198" t="s">
+      <c r="H7" s="199" t="s">
         <v>160</v>
       </c>
-      <c r="I7" s="198"/>
-      <c r="J7" s="198"/>
-      <c r="K7" s="198"/>
+      <c r="I7" s="199"/>
+      <c r="J7" s="199"/>
+      <c r="K7" s="199"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="202" t="s">
+      <c r="H8" s="203" t="s">
         <v>159</v>
       </c>
-      <c r="I8" s="202"/>
-      <c r="J8" s="202"/>
-      <c r="K8" s="202"/>
+      <c r="I8" s="203"/>
+      <c r="J8" s="203"/>
+      <c r="K8" s="203"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -14148,13 +14143,13 @@
         <f t="shared" si="68"/>
         <v>1.0918875794757976</v>
       </c>
-      <c r="E383" s="158">
+      <c r="E383" s="159">
         <v>2000</v>
       </c>
-      <c r="F383" s="160">
+      <c r="F383" s="161">
         <v>2000</v>
       </c>
-      <c r="G383" s="152">
+      <c r="G383" s="154">
         <f t="shared" si="69"/>
         <v>0.2105263157894737</v>
       </c>
@@ -14175,14 +14170,14 @@
         <v>1.2738688427217637</v>
       </c>
       <c r="E384" s="158">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F384" s="160">
         <v>5000</v>
       </c>
       <c r="G384" s="152">
         <f t="shared" si="69"/>
-        <v>8.4210526315789486E-2</v>
+        <v>0.84210526315789469</v>
       </c>
       <c r="I384" s="158">
         <v>3000</v>
@@ -14201,14 +14196,14 @@
         <v>1.45585010596773</v>
       </c>
       <c r="E385" s="158">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F385" s="160">
         <v>10000</v>
       </c>
       <c r="G385" s="152">
         <f t="shared" si="69"/>
-        <v>4.2105263157894743E-2</v>
+        <v>0.42105263157894735</v>
       </c>
       <c r="I385" s="158">
         <v>3500</v>
@@ -14227,14 +14222,14 @@
         <v>1.6378313692136963</v>
       </c>
       <c r="E386" s="158">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F386" s="160">
         <v>20000</v>
       </c>
       <c r="G386" s="152">
         <f t="shared" si="69"/>
-        <v>2.1052631578947371E-2</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="I386" s="158">
         <v>4000</v>
@@ -14253,14 +14248,14 @@
         <v>1.8198126324596626</v>
       </c>
       <c r="E387" s="158">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F387" s="160">
         <v>50000</v>
       </c>
       <c r="G387" s="152">
         <f t="shared" si="69"/>
-        <v>8.4210526315789472E-3</v>
+        <v>8.4210526315789472E-2</v>
       </c>
       <c r="I387" s="158">
         <v>4500</v>
@@ -14279,14 +14274,14 @@
         <v>2.0017938957056289</v>
       </c>
       <c r="E388" s="158">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F388" s="160">
         <v>100000</v>
       </c>
       <c r="G388" s="152">
         <f t="shared" si="69"/>
-        <v>4.2105263157894736E-3</v>
+        <v>4.2105263157894736E-2</v>
       </c>
       <c r="I388" s="158">
         <v>5000</v>
@@ -14305,14 +14300,14 @@
         <v>2.1837751589515952</v>
       </c>
       <c r="E389" s="159">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F389" s="161">
         <v>200000</v>
       </c>
       <c r="G389" s="154">
         <f t="shared" si="69"/>
-        <v>2.1052631578947368E-3</v>
+        <v>2.1052631578947368E-2</v>
       </c>
       <c r="I389" s="159">
         <v>5500</v>
@@ -14334,9 +14329,9 @@
       </c>
     </row>
     <row r="392" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A392" s="199"/>
-      <c r="B392" s="199"/>
-      <c r="C392" s="199"/>
+      <c r="A392" s="200"/>
+      <c r="B392" s="200"/>
+      <c r="C392" s="200"/>
       <c r="D392" s="5" t="s">
         <v>67</v>
       </c>
@@ -14354,11 +14349,11 @@
       </c>
     </row>
     <row r="393" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A393" s="201" t="s">
+      <c r="A393" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B393" s="201"/>
-      <c r="C393" s="201"/>
+      <c r="B393" s="202"/>
+      <c r="C393" s="202"/>
       <c r="D393" s="48" t="str">
         <f>A74</f>
         <v>90th %ile</v>
@@ -14378,11 +14373,11 @@
       <c r="H393" s="112"/>
     </row>
     <row r="394" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A394" s="200" t="s">
+      <c r="A394" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="B394" s="200"/>
-      <c r="C394" s="200"/>
+      <c r="B394" s="201"/>
+      <c r="C394" s="201"/>
       <c r="D394" s="2" t="str">
         <f>A50</f>
         <v>90th %ile</v>
@@ -14402,11 +14397,11 @@
       <c r="H394" s="109"/>
     </row>
     <row r="395" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A395" s="200" t="s">
+      <c r="A395" s="201" t="s">
         <v>49</v>
       </c>
-      <c r="B395" s="200"/>
-      <c r="C395" s="200"/>
+      <c r="B395" s="201"/>
+      <c r="C395" s="201"/>
       <c r="D395" s="2" t="str">
         <f>A258</f>
         <v>10th %ile</v>
@@ -14426,11 +14421,11 @@
       <c r="H395" s="109"/>
     </row>
     <row r="396" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A396" s="200" t="s">
+      <c r="A396" s="201" t="s">
         <v>66</v>
       </c>
-      <c r="B396" s="200"/>
-      <c r="C396" s="200"/>
+      <c r="B396" s="201"/>
+      <c r="C396" s="201"/>
       <c r="D396" s="2" t="str">
         <f>A283</f>
         <v>90th %ile</v>
@@ -14444,11 +14439,11 @@
       </c>
     </row>
     <row r="397" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A397" s="200" t="s">
+      <c r="A397" s="201" t="s">
         <v>71</v>
       </c>
-      <c r="B397" s="200"/>
-      <c r="C397" s="200"/>
+      <c r="B397" s="201"/>
+      <c r="C397" s="201"/>
       <c r="D397" s="2" t="str">
         <f>A98</f>
         <v>90th %ile</v>
@@ -14468,11 +14463,11 @@
       <c r="H397" s="109"/>
     </row>
     <row r="398" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A398" s="200" t="s">
+      <c r="A398" s="201" t="s">
         <v>56</v>
       </c>
-      <c r="B398" s="200"/>
-      <c r="C398" s="200"/>
+      <c r="B398" s="201"/>
+      <c r="C398" s="201"/>
       <c r="D398" s="2" t="str">
         <f>A162</f>
         <v>90th %ile</v>
@@ -14489,11 +14484,11 @@
       <c r="H398" s="109"/>
     </row>
     <row r="399" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A399" s="200" t="s">
+      <c r="A399" s="201" t="s">
         <v>54</v>
       </c>
-      <c r="B399" s="200"/>
-      <c r="C399" s="200"/>
+      <c r="B399" s="201"/>
+      <c r="C399" s="201"/>
       <c r="D399" s="2" t="str">
         <f>A210</f>
         <v>90th %ile</v>
@@ -14510,11 +14505,11 @@
       <c r="H399" s="109"/>
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A400" s="200" t="s">
+      <c r="A400" s="201" t="s">
         <v>47</v>
       </c>
-      <c r="B400" s="200"/>
-      <c r="C400" s="200"/>
+      <c r="B400" s="201"/>
+      <c r="C400" s="201"/>
       <c r="D400" s="2" t="str">
         <f>A234</f>
         <v>90th %ile</v>
@@ -14548,11 +14543,11 @@
       <c r="H401" s="175"/>
     </row>
     <row r="402" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A402" s="200" t="s">
+      <c r="A402" s="201" t="s">
         <v>56</v>
       </c>
-      <c r="B402" s="200"/>
-      <c r="C402" s="200"/>
+      <c r="B402" s="201"/>
+      <c r="C402" s="201"/>
       <c r="D402" s="95" t="s">
         <v>81</v>
       </c>
@@ -14685,8 +14680,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A284" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I313" sqref="I313"/>
+    <sheetView tabSelected="1" topLeftCell="A290" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17069,19 +17064,19 @@
       </c>
     </row>
     <row r="108" spans="1:8" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="201" t="s">
+      <c r="A108" s="202" t="s">
         <v>5</v>
       </c>
-      <c r="B108" s="201"/>
-      <c r="C108" s="201"/>
+      <c r="B108" s="202"/>
+      <c r="C108" s="202"/>
       <c r="D108" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="E108" s="105">
+      <c r="E108" s="198">
         <f>'Current Bitcoin'!E394</f>
         <v>0.8446313225664035</v>
       </c>
-      <c r="F108" s="203">
+      <c r="F108" s="198">
         <f>'Current Bitcoin'!F394/1000</f>
         <v>0.24071992693142499</v>
       </c>
@@ -17092,11 +17087,11 @@
       <c r="H108" s="109"/>
     </row>
     <row r="109" spans="1:8" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="200" t="s">
+      <c r="A109" s="201" t="s">
         <v>98</v>
       </c>
-      <c r="B109" s="200"/>
-      <c r="C109" s="200"/>
+      <c r="B109" s="201"/>
+      <c r="C109" s="201"/>
       <c r="D109" s="92" t="s">
         <v>80</v>
       </c>
@@ -17115,11 +17110,11 @@
       <c r="H109" s="109"/>
     </row>
     <row r="110" spans="1:8" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="201" t="s">
+      <c r="A110" s="202" t="s">
         <v>71</v>
       </c>
-      <c r="B110" s="201"/>
-      <c r="C110" s="201"/>
+      <c r="B110" s="202"/>
+      <c r="C110" s="202"/>
       <c r="D110" s="104" t="s">
         <v>80</v>
       </c>
@@ -17127,7 +17122,7 @@
         <f>'Current Bitcoin'!E397</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="F110" s="203">
+      <c r="F110" s="198">
         <f>'Current Bitcoin'!F397/1000</f>
         <v>1.3965000000000001</v>
       </c>
@@ -17138,11 +17133,11 @@
       <c r="H110" s="109"/>
     </row>
     <row r="111" spans="1:8" s="93" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="200" t="s">
+      <c r="A111" s="201" t="s">
         <v>97</v>
       </c>
-      <c r="B111" s="200"/>
-      <c r="C111" s="200"/>
+      <c r="B111" s="201"/>
+      <c r="C111" s="201"/>
       <c r="D111" s="92" t="s">
         <v>80</v>
       </c>
@@ -17160,11 +17155,11 @@
       <c r="H111" s="109"/>
     </row>
     <row r="112" spans="1:8" s="93" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="200" t="s">
+      <c r="A112" s="201" t="s">
         <v>92</v>
       </c>
-      <c r="B112" s="200"/>
-      <c r="C112" s="200"/>
+      <c r="B112" s="201"/>
+      <c r="C112" s="201"/>
       <c r="D112" s="92" t="s">
         <v>80</v>
       </c>
@@ -17182,11 +17177,11 @@
       <c r="H112" s="109"/>
     </row>
     <row r="113" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="200" t="s">
+      <c r="A113" s="201" t="s">
         <v>96</v>
       </c>
-      <c r="B113" s="200"/>
-      <c r="C113" s="200"/>
+      <c r="B113" s="201"/>
+      <c r="C113" s="201"/>
       <c r="D113" s="92" t="s">
         <v>80</v>
       </c>
@@ -21012,38 +21007,38 @@
         <v>0</v>
       </c>
       <c r="B260" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A260)*secondsPerBlock</f>
+        <f t="shared" ref="B260:B275" si="58">bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A260)*secondsPerBlock</f>
         <v>7.5</v>
       </c>
       <c r="C260" s="106">
-        <f>D260/(avgTrSize/(avgTrSize+D234))</f>
+        <f t="shared" ref="C260:C275" si="59">D260/(avgTrSize/(avgTrSize+D234))</f>
         <v>2420.289218527796</v>
       </c>
       <c r="D260" s="106">
-        <f>B260/neutrinoFilterRatio</f>
+        <f t="shared" ref="D260:D275" si="60">B260/neutrinoFilterRatio</f>
         <v>1000</v>
       </c>
       <c r="E260" s="87">
-        <f>D260*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" ref="E260:E275" si="61">D260*1000*1000/secondsPerBlock/avgTrSize</f>
         <v>3508.7719298245615</v>
       </c>
       <c r="G260" s="93">
         <v>0</v>
       </c>
       <c r="H260" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G260)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" ref="H260:H275" si="62">bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G260)*secondsPerYear*recentSyncTime16/365</f>
         <v>7560</v>
       </c>
       <c r="I260" s="106">
-        <f>J260/(avgTrSize/(avgTrSize+D234))</f>
+        <f t="shared" ref="I260:I275" si="63">J260/(avgTrSize/(avgTrSize+D234))</f>
         <v>80.676307284259877</v>
       </c>
       <c r="J260" s="106">
-        <f>secondsPerBlock*H260/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" ref="J260:J275" si="64">secondsPerBlock*H260/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
         <v>33.333333333333336</v>
       </c>
       <c r="K260" s="87">
-        <f>J260*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" ref="K260:K275" si="65">J260*1000*1000/secondsPerBlock/avgTrSize</f>
         <v>116.95906432748539</v>
       </c>
     </row>
@@ -21052,38 +21047,38 @@
         <v>1</v>
       </c>
       <c r="B261" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A261)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>9.375</v>
       </c>
       <c r="C261" s="106">
-        <f>D261/(avgTrSize/(avgTrSize+D235))</f>
+        <f t="shared" si="59"/>
         <v>3025.361523159745</v>
       </c>
       <c r="D261" s="106">
-        <f>B261/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>1250</v>
       </c>
       <c r="E261" s="87">
-        <f>D261*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>4385.9649122807014</v>
       </c>
       <c r="G261" s="93">
         <v>1</v>
       </c>
       <c r="H261" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G261)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>9450</v>
       </c>
       <c r="I261" s="106">
-        <f>J261/(avgTrSize/(avgTrSize+D235))</f>
+        <f t="shared" si="63"/>
         <v>100.84538410532484</v>
       </c>
       <c r="J261" s="106">
-        <f>secondsPerBlock*H261/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>41.666666666666671</v>
       </c>
       <c r="K261" s="87">
-        <f>J261*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>146.19883040935673</v>
       </c>
     </row>
@@ -21092,38 +21087,38 @@
         <v>2</v>
       </c>
       <c r="B262" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A262)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>11.71875</v>
       </c>
       <c r="C262" s="106">
-        <f>D262/(avgTrSize/(avgTrSize+D236))</f>
+        <f t="shared" si="59"/>
         <v>3781.7019039496813</v>
       </c>
       <c r="D262" s="106">
-        <f>B262/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>1562.5</v>
       </c>
       <c r="E262" s="87">
-        <f>D262*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>5482.4561403508769</v>
       </c>
       <c r="G262" s="93">
         <v>2</v>
       </c>
       <c r="H262" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G262)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>11812.5</v>
       </c>
       <c r="I262" s="106">
-        <f>J262/(avgTrSize/(avgTrSize+D236))</f>
+        <f t="shared" si="63"/>
         <v>126.05673013165605</v>
       </c>
       <c r="J262" s="106">
-        <f>secondsPerBlock*H262/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>52.083333333333336</v>
       </c>
       <c r="K262" s="87">
-        <f>J262*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>182.74853801169593</v>
       </c>
     </row>
@@ -21132,38 +21127,38 @@
         <v>3</v>
       </c>
       <c r="B263" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A263)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>14.6484375</v>
       </c>
       <c r="C263" s="106">
-        <f>D263/(avgTrSize/(avgTrSize+D237))</f>
+        <f t="shared" si="59"/>
         <v>4463.9694852002594</v>
       </c>
       <c r="D263" s="106">
-        <f>B263/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>1953.125</v>
       </c>
       <c r="E263" s="87">
-        <f>D263*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>6853.0701754385964</v>
       </c>
       <c r="G263" s="93">
         <v>3</v>
       </c>
       <c r="H263" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G263)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>14765.625</v>
       </c>
       <c r="I263" s="106">
-        <f>J263/(avgTrSize/(avgTrSize+D237))</f>
+        <f t="shared" si="63"/>
         <v>148.79898284000865</v>
       </c>
       <c r="J263" s="106">
-        <f>secondsPerBlock*H263/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>65.104166666666671</v>
       </c>
       <c r="K263" s="87">
-        <f>J263*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>228.43567251461991</v>
       </c>
     </row>
@@ -21172,38 +21167,38 @@
         <v>4</v>
       </c>
       <c r="B264" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A264)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>18.310546875</v>
       </c>
       <c r="C264" s="106">
-        <f>D264/(avgTrSize/(avgTrSize+D238))</f>
+        <f t="shared" si="59"/>
         <v>5579.9618565003238</v>
       </c>
       <c r="D264" s="106">
-        <f>B264/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>2441.40625</v>
       </c>
       <c r="E264" s="87">
-        <f>D264*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>8566.3377192982462</v>
       </c>
       <c r="G264" s="93">
         <v>4</v>
       </c>
       <c r="H264" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G264)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>18457.03125</v>
       </c>
       <c r="I264" s="106">
-        <f>J264/(avgTrSize/(avgTrSize+D238))</f>
+        <f t="shared" si="63"/>
         <v>185.99872855001084</v>
       </c>
       <c r="J264" s="106">
-        <f>secondsPerBlock*H264/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>81.380208333333343</v>
       </c>
       <c r="K264" s="87">
-        <f>J264*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>285.54459064327489</v>
       </c>
     </row>
@@ -21212,38 +21207,38 @@
         <v>5</v>
       </c>
       <c r="B265" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A265)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>22.88818359375</v>
       </c>
       <c r="C265" s="106">
-        <f>D265/(avgTrSize/(avgTrSize+D239))</f>
+        <f t="shared" si="59"/>
         <v>6974.9523206254053</v>
       </c>
       <c r="D265" s="106">
-        <f>B265/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>3051.7578125</v>
       </c>
       <c r="E265" s="87">
-        <f>D265*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>10707.922149122807</v>
       </c>
       <c r="G265" s="93">
         <v>5</v>
       </c>
       <c r="H265" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G265)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>23071.2890625</v>
       </c>
       <c r="I265" s="106">
-        <f>J265/(avgTrSize/(avgTrSize+D239))</f>
+        <f t="shared" si="63"/>
         <v>232.49841068751351</v>
       </c>
       <c r="J265" s="106">
-        <f>secondsPerBlock*H265/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>101.72526041666667</v>
       </c>
       <c r="K265" s="87">
-        <f>J265*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>356.93073830409361</v>
       </c>
     </row>
@@ -21252,38 +21247,38 @@
         <v>6</v>
       </c>
       <c r="B266" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A266)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>28.6102294921875</v>
       </c>
       <c r="C266" s="106">
-        <f>D266/(avgTrSize/(avgTrSize+D240))</f>
+        <f t="shared" si="59"/>
         <v>8718.6904007817575</v>
       </c>
       <c r="D266" s="106">
-        <f>B266/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>3814.697265625</v>
       </c>
       <c r="E266" s="87">
-        <f>D266*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>13384.90268640351</v>
       </c>
       <c r="G266" s="93">
         <v>6</v>
       </c>
       <c r="H266" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G266)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>28839.111328125</v>
       </c>
       <c r="I266" s="106">
-        <f>J266/(avgTrSize/(avgTrSize+D240))</f>
+        <f t="shared" si="63"/>
         <v>290.6230133593919</v>
       </c>
       <c r="J266" s="106">
-        <f>secondsPerBlock*H266/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>127.15657552083334</v>
       </c>
       <c r="K266" s="87">
-        <f>J266*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>446.16342288011697</v>
       </c>
     </row>
@@ -21292,38 +21287,38 @@
         <v>7</v>
       </c>
       <c r="B267" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A267)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>35.762786865234375</v>
       </c>
       <c r="C267" s="106">
-        <f>D267/(avgTrSize/(avgTrSize+D241))</f>
+        <f t="shared" si="59"/>
         <v>10898.363000977195</v>
       </c>
       <c r="D267" s="106">
-        <f>B267/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>4768.37158203125</v>
       </c>
       <c r="E267" s="87">
-        <f>D267*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>16731.128358004386</v>
       </c>
       <c r="G267" s="93">
         <v>7</v>
       </c>
       <c r="H267" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G267)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>36048.88916015625</v>
       </c>
       <c r="I267" s="106">
-        <f>J267/(avgTrSize/(avgTrSize+D241))</f>
+        <f t="shared" si="63"/>
         <v>363.2787666992399</v>
       </c>
       <c r="J267" s="106">
-        <f>secondsPerBlock*H267/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>158.94571940104169</v>
       </c>
       <c r="K267" s="87">
-        <f>J267*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>557.70427860014627</v>
       </c>
     </row>
@@ -21332,38 +21327,38 @@
         <v>8</v>
       </c>
       <c r="B268" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A268)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>44.703483581542969</v>
       </c>
       <c r="C268" s="106">
-        <f>D268/(avgTrSize/(avgTrSize+D242))</f>
+        <f t="shared" si="59"/>
         <v>12819.859590037284</v>
       </c>
       <c r="D268" s="106">
-        <f>B268/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>5960.4644775390625</v>
       </c>
       <c r="E268" s="87">
-        <f>D268*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>20913.910447505481</v>
       </c>
       <c r="G268" s="93">
         <v>8</v>
       </c>
       <c r="H268" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G268)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>45061.111450195313</v>
       </c>
       <c r="I268" s="106">
-        <f>J268/(avgTrSize/(avgTrSize+D242))</f>
+        <f t="shared" si="63"/>
         <v>427.32865300124286</v>
       </c>
       <c r="J268" s="106">
-        <f>secondsPerBlock*H268/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>198.68214925130209</v>
       </c>
       <c r="K268" s="87">
-        <f>J268*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>697.13034825018281</v>
       </c>
     </row>
@@ -21372,38 +21367,38 @@
         <v>9</v>
       </c>
       <c r="B269" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A269)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>55.879354476928711</v>
       </c>
       <c r="C269" s="106">
-        <f>D269/(avgTrSize/(avgTrSize+D243))</f>
+        <f t="shared" si="59"/>
         <v>16024.824487546606</v>
       </c>
       <c r="D269" s="106">
-        <f>B269/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>7450.5805969238281</v>
       </c>
       <c r="E269" s="87">
-        <f>D269*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>26142.388059381854</v>
       </c>
       <c r="G269" s="93">
         <v>9</v>
       </c>
       <c r="H269" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G269)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>56326.389312744141</v>
       </c>
       <c r="I269" s="106">
-        <f>J269/(avgTrSize/(avgTrSize+D243))</f>
+        <f t="shared" si="63"/>
         <v>534.16081625155357</v>
       </c>
       <c r="J269" s="106">
-        <f>secondsPerBlock*H269/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>248.35268656412762</v>
       </c>
       <c r="K269" s="87">
-        <f>J269*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>871.41293531272856</v>
       </c>
     </row>
@@ -21412,38 +21407,38 @@
         <v>10</v>
       </c>
       <c r="B270" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A270)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>69.849193096160889</v>
       </c>
       <c r="C270" s="106">
-        <f>D270/(avgTrSize/(avgTrSize+D244))</f>
+        <f t="shared" si="59"/>
         <v>20031.030609433255</v>
       </c>
       <c r="D270" s="106">
-        <f>B270/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>9313.2257461547852</v>
       </c>
       <c r="E270" s="87">
-        <f>D270*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>32677.985074227316</v>
       </c>
       <c r="G270" s="93">
         <v>10</v>
       </c>
       <c r="H270" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G270)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>70407.986640930176</v>
       </c>
       <c r="I270" s="106">
-        <f>J270/(avgTrSize/(avgTrSize+D244))</f>
+        <f t="shared" si="63"/>
         <v>667.70102031444196</v>
       </c>
       <c r="J270" s="106">
-        <f>secondsPerBlock*H270/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>310.44085820515954</v>
       </c>
       <c r="K270" s="87">
-        <f>J270*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>1089.2661691409107</v>
       </c>
     </row>
@@ -21452,38 +21447,38 @@
         <v>11</v>
       </c>
       <c r="B271" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A271)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>87.311491370201111</v>
       </c>
       <c r="C271" s="106">
-        <f>D271/(avgTrSize/(avgTrSize+D245))</f>
+        <f t="shared" si="59"/>
         <v>25038.788261791571</v>
       </c>
       <c r="D271" s="106">
-        <f>B271/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>11641.532182693481</v>
       </c>
       <c r="E271" s="87">
-        <f>D271*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>40847.481342784144</v>
       </c>
       <c r="G271" s="93">
         <v>11</v>
       </c>
       <c r="H271" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G271)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>88009.98330116272</v>
       </c>
       <c r="I271" s="106">
-        <f>J271/(avgTrSize/(avgTrSize+D245))</f>
+        <f t="shared" si="63"/>
         <v>834.62627539305242</v>
       </c>
       <c r="J271" s="106">
-        <f>secondsPerBlock*H271/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>388.0510727564494</v>
       </c>
       <c r="K271" s="87">
-        <f>J271*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>1361.5827114261383</v>
       </c>
     </row>
@@ -21492,38 +21487,38 @@
         <v>12</v>
       </c>
       <c r="B272" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A272)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>109.13936421275139</v>
       </c>
       <c r="C272" s="106">
-        <f>D272/(avgTrSize/(avgTrSize+D246))</f>
+        <f t="shared" si="59"/>
         <v>31298.485327239465</v>
       </c>
       <c r="D272" s="106">
-        <f>B272/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>14551.915228366852</v>
       </c>
       <c r="E272" s="87">
-        <f>D272*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>51059.351678480183</v>
       </c>
       <c r="G272" s="93">
         <v>12</v>
       </c>
       <c r="H272" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G272)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>110012.4791264534</v>
       </c>
       <c r="I272" s="106">
-        <f>J272/(avgTrSize/(avgTrSize+D246))</f>
+        <f t="shared" si="63"/>
         <v>1043.2828442413156</v>
       </c>
       <c r="J272" s="106">
-        <f>secondsPerBlock*H272/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>485.06384094556176</v>
       </c>
       <c r="K272" s="87">
-        <f>J272*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>1701.9783892826729</v>
       </c>
     </row>
@@ -21532,38 +21527,38 @@
         <v>13</v>
       </c>
       <c r="B273" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A273)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>136.42420526593924</v>
       </c>
       <c r="C273" s="106">
-        <f>D273/(avgTrSize/(avgTrSize+D247))</f>
+        <f t="shared" si="59"/>
         <v>36672.257778482286</v>
       </c>
       <c r="D273" s="106">
-        <f>B273/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>18189.894035458565</v>
       </c>
       <c r="E273" s="87">
-        <f>D273*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>63824.189598100224</v>
       </c>
       <c r="G273" s="93">
         <v>13</v>
       </c>
       <c r="H273" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G273)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>137515.59890806675</v>
       </c>
       <c r="I273" s="106">
-        <f>J273/(avgTrSize/(avgTrSize+D247))</f>
+        <f t="shared" si="63"/>
         <v>1222.4085926160762</v>
       </c>
       <c r="J273" s="106">
-        <f>secondsPerBlock*H273/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>606.32980118195223</v>
       </c>
       <c r="K273" s="87">
-        <f>J273*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>2127.4729866033413</v>
       </c>
     </row>
@@ -21572,38 +21567,38 @@
         <v>14</v>
       </c>
       <c r="B274" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A274)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>170.53025658242404</v>
       </c>
       <c r="C274" s="106">
-        <f>D274/(avgTrSize/(avgTrSize+D248))</f>
+        <f t="shared" si="59"/>
         <v>45840.322223102856</v>
       </c>
       <c r="D274" s="106">
-        <f>B274/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>22737.367544323206</v>
       </c>
       <c r="E274" s="87">
-        <f>D274*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>79780.236997625281</v>
       </c>
       <c r="G274" s="93">
         <v>14</v>
       </c>
       <c r="H274" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G274)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>171894.49863508344</v>
       </c>
       <c r="I274" s="106">
-        <f>J274/(avgTrSize/(avgTrSize+D248))</f>
+        <f t="shared" si="63"/>
         <v>1528.0107407700953</v>
       </c>
       <c r="J274" s="106">
-        <f>secondsPerBlock*H274/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>757.91225147744024</v>
       </c>
       <c r="K274" s="87">
-        <f>J274*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>2659.3412332541766</v>
       </c>
     </row>
@@ -21612,38 +21607,38 @@
         <v>15</v>
       </c>
       <c r="B275" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,A275)*secondsPerBlock</f>
+        <f t="shared" si="58"/>
         <v>213.16282072803006</v>
       </c>
       <c r="C275" s="106">
-        <f>D275/(avgTrSize/(avgTrSize+D249))</f>
+        <f t="shared" si="59"/>
         <v>57300.402778878568</v>
       </c>
       <c r="D275" s="106">
-        <f>B275/neutrinoFilterRatio</f>
+        <f t="shared" si="60"/>
         <v>28421.709430404007</v>
       </c>
       <c r="E275" s="87">
-        <f>D275*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="61"/>
         <v>99725.296247031612</v>
       </c>
       <c r="G275" s="93">
         <v>15</v>
       </c>
       <c r="H275" s="42">
-        <f>bandwidth16*ongoingResourcePercentage16*mbToGB*1000*POWER(1+bandwidthGrowth,G275)*secondsPerYear*recentSyncTime16/365</f>
+        <f t="shared" si="62"/>
         <v>214868.12329385427</v>
       </c>
       <c r="I275" s="106">
-        <f>J275/(avgTrSize/(avgTrSize+D249))</f>
+        <f t="shared" si="63"/>
         <v>1910.0134259626188</v>
       </c>
       <c r="J275" s="106">
-        <f>secondsPerBlock*H275/(secondsPerYear*assumevalidBlockTime/365)/neutrinoFilterRatio</f>
+        <f t="shared" si="64"/>
         <v>947.39031434680021</v>
       </c>
       <c r="K275" s="87">
-        <f>J275*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" si="65"/>
         <v>3324.1765415677196</v>
       </c>
     </row>
@@ -22056,7 +22051,7 @@
         <v>0</v>
       </c>
       <c r="B292" s="133">
-        <f t="shared" ref="B292:B307" si="58">secondsPerBlock*maximumMinerAdvantage2/targetMinerPercentHashpower2</f>
+        <f t="shared" ref="B292:B307" si="66">secondsPerBlock*maximumMinerAdvantage2/targetMinerPercentHashpower2</f>
         <v>2.4</v>
       </c>
       <c r="C292" s="172">
@@ -22064,11 +22059,11 @@
         <v>0.38890982298128057</v>
       </c>
       <c r="D292" s="106">
-        <f t="shared" ref="D292:D307" si="59">(B292 - C292)*(avgLowRelayBandwidth*ongoingResourcePercent10thP2*POWER(1+bandwidthGrowth,A292)*mbToGB*1000)/(compactBlockCompactedness+missingTransactionRate)</f>
+        <f t="shared" ref="D292:D307" si="67">(B292 - C292)*(avgLowRelayBandwidth*ongoingResourcePercent10thP2*POWER(1+bandwidthGrowth,A292)*mbToGB*1000)/(compactBlockCompactedness+missingTransactionRate)</f>
         <v>66.154282138773667</v>
       </c>
       <c r="E292" s="106">
-        <f>(B292 - C292)*(avgTrSize+D234)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A292))/missingTransactionRate/1000/1000</f>
+        <f t="shared" ref="E292:E307" si="68">(B292 - C292)*(avgTrSize+D234)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A292))/missingTransactionRate/1000/1000</f>
         <v>115.60122198198215</v>
       </c>
       <c r="F292" s="106">
@@ -22076,7 +22071,7 @@
         <v>66.154282138773667</v>
       </c>
       <c r="G292" s="106">
-        <f>F292*endGameTransactionSize/(endGameTransactionSize+D234)</f>
+        <f t="shared" ref="G292:G307" si="69">F292*endGameTransactionSize/(endGameTransactionSize+D234)</f>
         <v>27.333213581397406</v>
       </c>
       <c r="H292" s="6">
@@ -22084,15 +22079,15 @@
         <v>95.906012566306686</v>
       </c>
       <c r="I292" s="136">
-        <f t="shared" ref="I292:I307" si="60">F292*(missingTransactionRate+compactBlockCompactedness)/(avgLowRelayBandwidth*ongoingResourcePercent10thP2*POWER(1+bandwidthGrowth,A292)*mbToGB*1000)</f>
+        <f t="shared" ref="I292:I307" si="70">F292*(missingTransactionRate+compactBlockCompactedness)/(avgLowRelayBandwidth*ongoingResourcePercent10thP2*POWER(1+bandwidthGrowth,A292)*mbToGB*1000)</f>
         <v>2.0110901770187195</v>
       </c>
       <c r="J292" s="137">
-        <f t="shared" ref="J292:J307" si="61">(G292*missingTransactionRate*1000*1000/avgTrSize)/(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A292))</f>
+        <f t="shared" ref="J292:J307" si="71">(G292*missingTransactionRate*1000*1000/avgTrSize)/(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A292))</f>
         <v>1.1508721507956803</v>
       </c>
       <c r="K292" s="180">
-        <f t="shared" ref="K292:K306" si="62">MAX(I292,J292)+C292</f>
+        <f t="shared" ref="K292:K306" si="72">MAX(I292,J292)+C292</f>
         <v>2.4</v>
       </c>
     </row>
@@ -22101,43 +22096,43 @@
         <v>1</v>
       </c>
       <c r="B293" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C293" s="172">
-        <f t="shared" ref="C293:C307" si="63">(((avgHops20-1)*minLastMileLatency) + ((avgHops20-1)*proximityFavoringFactor2*(Latency1stP2-minLastMileLatency)+(Latency10thP2-minLastMileLatency))*(1-(1-POWER(1+latencyGrowth,A293))))/1000</f>
+        <f t="shared" ref="C293:C307" si="73">(((avgHops20-1)*minLastMileLatency) + ((avgHops20-1)*proximityFavoringFactor2*(Latency1stP2-minLastMileLatency)+(Latency10thP2-minLastMileLatency))*(1-(1-POWER(1+latencyGrowth,A293))))/1000</f>
         <v>0.3795903267745388</v>
       </c>
       <c r="D293" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>83.076055642494282</v>
       </c>
       <c r="E293" s="106">
-        <f>(B293 - C293)*(avgTrSize+D235)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A293))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>135.8802011285845</v>
       </c>
       <c r="F293" s="106">
-        <f t="shared" ref="F293:F307" si="64">MIN(D293,E293)</f>
+        <f t="shared" ref="F293:F307" si="74">MIN(D293,E293)</f>
         <v>83.076055642494282</v>
       </c>
       <c r="G293" s="106">
-        <f>F293*endGameTransactionSize/(endGameTransactionSize+D235)</f>
+        <f t="shared" si="69"/>
         <v>34.324846388824334</v>
       </c>
       <c r="H293" s="6">
-        <f t="shared" ref="H293:H307" si="65">G293*1000*1000/secondsPerBlock/avgTrSize</f>
+        <f t="shared" ref="H293:H307" si="75">G293*1000*1000/secondsPerBlock/avgTrSize</f>
         <v>120.43805750464679</v>
       </c>
       <c r="I293" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>2.0204096732254611</v>
       </c>
       <c r="J293" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>1.2352621282527874</v>
       </c>
       <c r="K293" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22146,43 +22141,43 @@
         <v>2</v>
       </c>
       <c r="B294" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C294" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.37055041545399936</v>
       </c>
       <c r="D294" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>104.30970315306335</v>
       </c>
       <c r="E294" s="106">
-        <f>(B294 - C294)*(avgTrSize+D236)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A294))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>159.69115819327311</v>
       </c>
       <c r="F294" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>104.30970315306335</v>
       </c>
       <c r="G294" s="106">
-        <f>F294*endGameTransactionSize/(endGameTransactionSize+D236)</f>
+        <f t="shared" si="69"/>
         <v>43.098032398174482</v>
       </c>
       <c r="H294" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>151.22116630938413</v>
       </c>
       <c r="I294" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>2.0294495845460006</v>
       </c>
       <c r="J294" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>1.3256293342922125</v>
       </c>
       <c r="K294" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22191,43 +22186,43 @@
         <v>3</v>
       </c>
       <c r="B295" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C295" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.36178170147307603</v>
       </c>
       <c r="D295" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>130.95049718126307</v>
       </c>
       <c r="E295" s="106">
-        <f>(B295 - C295)*(avgTrSize+D237)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A295))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>177.19973725847595</v>
       </c>
       <c r="F295" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>130.95049718126307</v>
       </c>
       <c r="G295" s="106">
-        <f>F295*endGameTransactionSize/(endGameTransactionSize+D237)</f>
+        <f t="shared" si="69"/>
         <v>57.294901019172308</v>
       </c>
       <c r="H295" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>201.03474041814843</v>
       </c>
       <c r="I295" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>2.0382182985269237</v>
       </c>
       <c r="J295" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>1.5062420728464254</v>
       </c>
       <c r="K295" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22236,43 +22231,43 @@
         <v>4</v>
       </c>
       <c r="B296" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C296" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.35327604891158049</v>
       </c>
       <c r="D296" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>164.37120546749875</v>
       </c>
       <c r="E296" s="106">
-        <f>(B296 - C296)*(avgTrSize+D238)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A296))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>208.18887140973581</v>
       </c>
       <c r="F296" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>164.37120546749875</v>
       </c>
       <c r="G296" s="106">
-        <f>F296*endGameTransactionSize/(endGameTransactionSize+D238)</f>
+        <f t="shared" si="69"/>
         <v>71.917496690573003</v>
       </c>
       <c r="H296" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>252.34209365113333</v>
       </c>
       <c r="I296" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>2.0467239510884196</v>
       </c>
       <c r="J296" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>1.6159484453782043</v>
       </c>
       <c r="K296" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -22281,43 +22276,43 @@
         <v>5</v>
       </c>
       <c r="B297" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C297" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.34502556592692973</v>
       </c>
       <c r="D297" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>206.29224617336374</v>
       </c>
       <c r="E297" s="106">
-        <f>(B297 - C297)*(avgTrSize+D239)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A297))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>244.56287098916613</v>
       </c>
       <c r="F297" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>206.29224617336374</v>
       </c>
       <c r="G297" s="106">
-        <f>F297*endGameTransactionSize/(endGameTransactionSize+D239)</f>
+        <f t="shared" si="69"/>
         <v>90.259251243352935</v>
       </c>
       <c r="H297" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>316.69912716965945</v>
       </c>
       <c r="I297" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>2.05497443407307</v>
       </c>
       <c r="J297" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>1.7334000460460328</v>
       </c>
       <c r="K297" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22326,43 +22321,43 @@
         <v>6</v>
       </c>
       <c r="B298" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C298" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.33702259743181856</v>
       </c>
       <c r="D298" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>258.8695479152305</v>
       </c>
       <c r="E298" s="106">
-        <f>(B298 - C298)*(avgTrSize+D240)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A298))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>287.25290765232546</v>
       </c>
       <c r="F298" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>258.8695479152305</v>
       </c>
       <c r="G298" s="106">
-        <f>F298*endGameTransactionSize/(endGameTransactionSize+D240)</f>
+        <f t="shared" si="69"/>
         <v>113.26345026510693</v>
       </c>
       <c r="H298" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>397.41561496528743</v>
       </c>
       <c r="I298" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>2.0629774025681815</v>
       </c>
       <c r="J298" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>1.8591353240835971</v>
       </c>
       <c r="K298" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22371,43 +22366,43 @@
         <v>7</v>
       </c>
       <c r="B299" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C299" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.32925971799156073</v>
       </c>
       <c r="D299" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>324.80457613475056</v>
       </c>
       <c r="E299" s="106">
-        <f>(B299 - C299)*(avgTrSize+D241)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A299))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>337.35057617368727</v>
       </c>
       <c r="F299" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>324.80457613475056</v>
       </c>
       <c r="G299" s="106">
-        <f>F299*endGameTransactionSize/(endGameTransactionSize+D241)</f>
+        <f t="shared" si="69"/>
         <v>142.11206861211897</v>
       </c>
       <c r="H299" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>498.63883723550526</v>
       </c>
       <c r="I299" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>2.0707402820084391</v>
       </c>
       <c r="J299" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>1.9937298676395898</v>
       </c>
       <c r="K299" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22416,43 +22411,43 @@
         <v>8</v>
       </c>
       <c r="B300" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C300" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.32172972493451052</v>
       </c>
       <c r="D300" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>407.48211017280215</v>
       </c>
       <c r="E300" s="106">
-        <f>(B300 - C300)*(avgTrSize+D242)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A300))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>372.78265620680645</v>
       </c>
       <c r="F300" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>372.78265620680645</v>
       </c>
       <c r="G300" s="106">
-        <f>F300*endGameTransactionSize/(endGameTransactionSize+D242)</f>
+        <f t="shared" si="69"/>
         <v>173.32153792776947</v>
       </c>
       <c r="H300" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>608.14574711498074</v>
       </c>
       <c r="I300" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.901293563847541</v>
       </c>
       <c r="J300" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.0782702750654893</v>
       </c>
       <c r="K300" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22461,43 +22456,43 @@
         <v>9</v>
       </c>
       <c r="B301" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C301" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.31442563166917192</v>
       </c>
       <c r="D301" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>511.1427605962939</v>
       </c>
       <c r="E301" s="106">
-        <f>(B301 - C301)*(avgTrSize+D243)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A301))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>437.68857959577861</v>
       </c>
       <c r="F301" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>437.68857959577861</v>
       </c>
       <c r="G301" s="106">
-        <f>F301*endGameTransactionSize/(endGameTransactionSize+D243)</f>
+        <f t="shared" si="69"/>
         <v>203.49889268152114</v>
       </c>
       <c r="H301" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>714.03120239130226</v>
       </c>
       <c r="I301" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.785865228436734</v>
       </c>
       <c r="J301" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.0855743683308283</v>
       </c>
       <c r="K301" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -22506,43 +22501,43 @@
         <v>10</v>
       </c>
       <c r="B302" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C302" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.30734066120179343</v>
       </c>
       <c r="D302" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>641.09897473772071</v>
       </c>
       <c r="E302" s="106">
-        <f>(B302 - C302)*(avgTrSize+D244)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A302))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>513.83529437125776</v>
       </c>
       <c r="F302" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>513.83529437125776</v>
       </c>
       <c r="G302" s="106">
-        <f>F302*endGameTransactionSize/(endGameTransactionSize+D244)</f>
+        <f t="shared" si="69"/>
         <v>238.90254007039417</v>
       </c>
       <c r="H302" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>838.25452656278651</v>
       </c>
       <c r="I302" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.6772483964898646</v>
       </c>
       <c r="J302" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.0926593387982062</v>
       </c>
       <c r="K302" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.3999999999999995</v>
       </c>
     </row>
@@ -22551,43 +22546,43 @@
         <v>11</v>
       </c>
       <c r="B303" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C303" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.30046823984843635</v>
       </c>
       <c r="D303" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>804.00547876287897</v>
       </c>
       <c r="E303" s="106">
-        <f>(B303 - C303)*(avgTrSize+D245)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A303))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>603.16163028591052</v>
       </c>
       <c r="F303" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>603.16163028591052</v>
       </c>
       <c r="G303" s="106">
-        <f>F303*endGameTransactionSize/(endGameTransactionSize+D245)</f>
+        <f t="shared" si="69"/>
         <v>280.43391944226926</v>
       </c>
       <c r="H303" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>983.97866470971667</v>
       </c>
       <c r="I303" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.5750601615782576</v>
       </c>
       <c r="J303" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.0995317601515637</v>
       </c>
       <c r="K303" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22596,43 +22591,43 @@
         <v>12</v>
       </c>
       <c r="B304" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C304" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.29380199113567995</v>
       </c>
       <c r="D304" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>1008.1978578667315</v>
       </c>
       <c r="E304" s="106">
-        <f>(B304 - C304)*(avgTrSize+D246)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A304))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>707.93978121512487</v>
       </c>
       <c r="F304" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>707.93978121512487</v>
       </c>
       <c r="G304" s="106">
-        <f>F304*endGameTransactionSize/(endGameTransactionSize+D246)</f>
+        <f t="shared" si="69"/>
         <v>329.14946443319468</v>
       </c>
       <c r="H304" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>1154.9104015199812</v>
       </c>
       <c r="I304" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.4789372403013317</v>
       </c>
       <c r="J304" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.10619800886432</v>
       </c>
       <c r="K304" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22641,43 +22636,43 @@
         <v>13</v>
       </c>
       <c r="B305" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C305" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.28733572988430622</v>
       </c>
       <c r="D305" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>1264.1164212468384</v>
       </c>
       <c r="E305" s="106">
-        <f>(B305 - C305)*(avgTrSize+D247)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A305))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>778.78536883613913</v>
       </c>
       <c r="F305" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>778.78536883613913</v>
       </c>
       <c r="G305" s="106">
-        <f>F305*endGameTransactionSize/(endGameTransactionSize+D247)</f>
+        <f t="shared" si="69"/>
         <v>386.28718801728388</v>
       </c>
       <c r="H305" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>1355.3936421659082</v>
       </c>
       <c r="I305" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.301551024237277</v>
       </c>
       <c r="J305" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.1126642701156944</v>
       </c>
       <c r="K305" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -22686,43 +22681,43 @@
         <v>14</v>
       </c>
       <c r="B306" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C306" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.28106345647047376</v>
       </c>
       <c r="D306" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>1584.8368089910737</v>
       </c>
       <c r="E306" s="106">
-        <f>(B306 - C306)*(avgTrSize+D248)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A306))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>913.88407381836271</v>
       </c>
       <c r="F306" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>913.88407381836271</v>
       </c>
       <c r="G306" s="106">
-        <f>F306*endGameTransactionSize/(endGameTransactionSize+D248)</f>
+        <f t="shared" si="69"/>
         <v>453.29781885431515</v>
       </c>
       <c r="H306" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>1590.51866264672</v>
       </c>
       <c r="I306" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.2218686173727495</v>
       </c>
       <c r="J306" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.118936543529526</v>
       </c>
       <c r="K306" s="180">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>2.4</v>
       </c>
     </row>
@@ -22731,39 +22726,39 @@
         <v>15</v>
       </c>
       <c r="B307" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="66"/>
         <v>2.4</v>
       </c>
       <c r="C307" s="172">
-        <f t="shared" si="63"/>
+        <f t="shared" si="73"/>
         <v>0.2749793512590562</v>
       </c>
       <c r="D307" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="67"/>
         <v>1986.7341911882802</v>
       </c>
       <c r="E307" s="106">
-        <f>(B307 - C307)*(avgTrSize+D249)*(avgLowRelayVerification*ongoingResourcePercent10thP2*POWER(1+cpuGrowth,A307))/missingTransactionRate/1000/1000</f>
+        <f t="shared" si="68"/>
         <v>1072.3144890861472</v>
       </c>
       <c r="F307" s="106">
-        <f t="shared" si="64"/>
+        <f t="shared" si="74"/>
         <v>1072.3144890861472</v>
       </c>
       <c r="G307" s="106">
-        <f>F307*endGameTransactionSize/(endGameTransactionSize+D249)</f>
+        <f t="shared" si="69"/>
         <v>531.88126695075698</v>
       </c>
       <c r="H307" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="75"/>
         <v>1866.2500594763403</v>
       </c>
       <c r="I307" s="136">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>1.1469528441996846</v>
       </c>
       <c r="J307" s="137">
-        <f t="shared" si="61"/>
+        <f t="shared" si="71"/>
         <v>2.1250206487409438</v>
       </c>
       <c r="K307" s="180">
@@ -22826,7 +22821,7 @@
         <v>40</v>
       </c>
       <c r="C311" s="152">
-        <f t="shared" ref="C311:C321" si="66">(avgHops19)*B311/1000</f>
+        <f t="shared" ref="C311:C321" si="76">(avgHops19)*B311/1000</f>
         <v>0.20396252649193253</v>
       </c>
       <c r="E311" s="158">
@@ -22836,14 +22831,14 @@
         <v>100</v>
       </c>
       <c r="G311" s="152">
-        <f t="shared" ref="G311:G321" si="67">(E311*missingTransactionRate*1000/avgTrSize)/(F311*ongoingResourcePercent10thP2)</f>
+        <f t="shared" ref="G311:G321" si="77">(E311*missingTransactionRate*1000/avgTrSize)/(F311*ongoingResourcePercent10thP2)</f>
         <v>10.526315789473683</v>
       </c>
       <c r="I311" s="158">
         <v>500</v>
       </c>
       <c r="J311" s="152">
-        <f t="shared" ref="J311:J321" si="68">I311*(missingTransactionRate+compactBlockCompactedness)/(avgRelayBandwidth*ongoingResourcePercent10thP2*mbToGB*KBperGB)</f>
+        <f t="shared" ref="J311:J321" si="78">I311*(missingTransactionRate+compactBlockCompactedness)/(avgRelayBandwidth*ongoingResourcePercent10thP2*mbToGB*KBperGB)</f>
         <v>1.52E-2</v>
       </c>
     </row>
@@ -22852,7 +22847,7 @@
         <v>60</v>
       </c>
       <c r="C312" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>0.30594378973789876</v>
       </c>
       <c r="E312" s="158">
@@ -22862,14 +22857,14 @@
         <v>200</v>
       </c>
       <c r="G312" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>5.2631578947368416</v>
       </c>
       <c r="I312" s="158">
         <v>1000</v>
       </c>
       <c r="J312" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>3.04E-2</v>
       </c>
     </row>
@@ -22878,7 +22873,7 @@
         <v>80</v>
       </c>
       <c r="C313" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>0.40792505298386506</v>
       </c>
       <c r="E313" s="158">
@@ -22888,14 +22883,14 @@
         <v>500</v>
       </c>
       <c r="G313" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>2.1052631578947367</v>
       </c>
       <c r="I313" s="158">
         <v>1500</v>
       </c>
       <c r="J313" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>4.5600000000000002E-2</v>
       </c>
     </row>
@@ -22904,7 +22899,7 @@
         <v>100</v>
       </c>
       <c r="C314" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>0.50990631622983129</v>
       </c>
       <c r="E314" s="158">
@@ -22914,14 +22909,14 @@
         <v>1000</v>
       </c>
       <c r="G314" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>1.0526315789473684</v>
       </c>
       <c r="I314" s="158">
         <v>2000</v>
       </c>
       <c r="J314" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>6.08E-2</v>
       </c>
     </row>
@@ -22930,7 +22925,7 @@
         <v>120</v>
       </c>
       <c r="C315" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>0.61188757947579753</v>
       </c>
       <c r="E315" s="158">
@@ -22940,14 +22935,14 @@
         <v>2000</v>
       </c>
       <c r="G315" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>0.52631578947368418</v>
       </c>
       <c r="I315" s="158">
         <v>2500</v>
       </c>
       <c r="J315" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
@@ -22956,7 +22951,7 @@
         <v>140</v>
       </c>
       <c r="C316" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>0.71386884272176387</v>
       </c>
       <c r="E316" s="158">
@@ -22966,14 +22961,14 @@
         <v>5000</v>
       </c>
       <c r="G316" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>0.21052631578947367</v>
       </c>
       <c r="I316" s="158">
         <v>3000</v>
       </c>
       <c r="J316" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>9.1200000000000003E-2</v>
       </c>
     </row>
@@ -22982,7 +22977,7 @@
         <v>160</v>
       </c>
       <c r="C317" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>0.81585010596773011</v>
       </c>
       <c r="E317" s="158">
@@ -22992,14 +22987,14 @@
         <v>10000</v>
       </c>
       <c r="G317" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>0.10526315789473684</v>
       </c>
       <c r="I317" s="158">
         <v>3500</v>
       </c>
       <c r="J317" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>0.10639999999999999</v>
       </c>
     </row>
@@ -23008,7 +23003,7 @@
         <v>180</v>
       </c>
       <c r="C318" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>0.91783136921369624</v>
       </c>
       <c r="E318" s="158">
@@ -23018,14 +23013,14 @@
         <v>20000</v>
       </c>
       <c r="G318" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="I318" s="158">
         <v>4000</v>
       </c>
       <c r="J318" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>0.1216</v>
       </c>
     </row>
@@ -23034,7 +23029,7 @@
         <v>200</v>
       </c>
       <c r="C319" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>1.0198126324596626</v>
       </c>
       <c r="E319" s="158">
@@ -23044,14 +23039,14 @@
         <v>50000</v>
       </c>
       <c r="G319" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>2.1052631578947368E-2</v>
       </c>
       <c r="I319" s="158">
         <v>4500</v>
       </c>
       <c r="J319" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>0.1368</v>
       </c>
     </row>
@@ -23060,7 +23055,7 @@
         <v>220</v>
       </c>
       <c r="C320" s="152">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>1.1217938957056288</v>
       </c>
       <c r="E320" s="158">
@@ -23070,14 +23065,14 @@
         <v>100000</v>
       </c>
       <c r="G320" s="152">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="I320" s="158">
         <v>5000</v>
       </c>
       <c r="J320" s="152">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>0.152</v>
       </c>
     </row>
@@ -23086,7 +23081,7 @@
         <v>240</v>
       </c>
       <c r="C321" s="154">
-        <f t="shared" si="66"/>
+        <f t="shared" si="76"/>
         <v>1.2237751589515951</v>
       </c>
       <c r="E321" s="159">
@@ -23096,14 +23091,14 @@
         <v>200000</v>
       </c>
       <c r="G321" s="154">
-        <f t="shared" si="67"/>
+        <f t="shared" si="77"/>
         <v>5.263157894736842E-3</v>
       </c>
       <c r="I321" s="159">
         <v>5500</v>
       </c>
       <c r="J321" s="154">
-        <f t="shared" si="68"/>
+        <f t="shared" si="78"/>
         <v>0.16719999999999999</v>
       </c>
     </row>
@@ -23202,7 +23197,7 @@
         <v>182</v>
       </c>
       <c r="E333" s="92" t="str">
-        <f t="shared" ref="E333:E341" si="69">$A$118</f>
+        <f t="shared" ref="E333:E341" si="79">$A$118</f>
         <v>10th %ile</v>
       </c>
       <c r="F333" s="185">
@@ -23221,7 +23216,7 @@
         <v>4</v>
       </c>
       <c r="J333" s="178">
-        <f t="shared" ref="J333:K358" si="70">endGameUsers*utxosPerUserEndGame</f>
+        <f t="shared" ref="J333:J355" si="80">endGameUsers*utxosPerUserEndGame</f>
         <v>800</v>
       </c>
     </row>
@@ -23230,7 +23225,7 @@
         <v>181</v>
       </c>
       <c r="E334" s="92" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="79"/>
         <v>10th %ile</v>
       </c>
       <c r="F334" s="87">
@@ -23249,7 +23244,7 @@
         <v>4</v>
       </c>
       <c r="J334" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23276,7 +23271,7 @@
         <v>4</v>
       </c>
       <c r="J335" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23305,7 +23300,7 @@
         <v>4</v>
       </c>
       <c r="J336" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23314,7 +23309,7 @@
         <v>123</v>
       </c>
       <c r="E337" s="92" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="79"/>
         <v>10th %ile</v>
       </c>
       <c r="F337" s="185">
@@ -23333,7 +23328,7 @@
         <v>4</v>
       </c>
       <c r="J337" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23342,7 +23337,7 @@
         <v>189</v>
       </c>
       <c r="E338" s="92" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="79"/>
         <v>10th %ile</v>
       </c>
       <c r="F338" s="185">
@@ -23361,7 +23356,7 @@
         <v>4</v>
       </c>
       <c r="J338" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23389,7 +23384,7 @@
         <v>4</v>
       </c>
       <c r="J339" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23398,7 +23393,7 @@
         <v>191</v>
       </c>
       <c r="E340" s="92" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="79"/>
         <v>10th %ile</v>
       </c>
       <c r="F340" s="185">
@@ -23417,7 +23412,7 @@
         <v>4</v>
       </c>
       <c r="J340" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23429,7 +23424,7 @@
         <v>192</v>
       </c>
       <c r="E341" s="92" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="79"/>
         <v>10th %ile</v>
       </c>
       <c r="F341" s="185">
@@ -23448,7 +23443,7 @@
         <v>4</v>
       </c>
       <c r="J341" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23526,7 +23521,7 @@
         <v>182</v>
       </c>
       <c r="E347" s="92" t="str">
-        <f t="shared" ref="E347:E354" si="71">$A$118</f>
+        <f t="shared" ref="E347:E354" si="81">$A$118</f>
         <v>10th %ile</v>
       </c>
       <c r="F347" s="185">
@@ -23545,7 +23540,7 @@
         <v>4</v>
       </c>
       <c r="J347" s="178">
-        <f t="shared" ref="J347:J354" si="72">endGameUsers*utxosPerUserEndGame</f>
+        <f t="shared" ref="J347:J354" si="82">endGameUsers*utxosPerUserEndGame</f>
         <v>800</v>
       </c>
     </row>
@@ -23575,7 +23570,7 @@
         <v>4</v>
       </c>
       <c r="J348" s="178">
-        <f t="shared" si="72"/>
+        <f t="shared" si="82"/>
         <v>800</v>
       </c>
     </row>
@@ -23585,7 +23580,7 @@
         <v>181</v>
       </c>
       <c r="E349" s="92" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="81"/>
         <v>10th %ile</v>
       </c>
       <c r="F349" s="87">
@@ -23604,7 +23599,7 @@
         <v>4</v>
       </c>
       <c r="J349" s="178">
-        <f t="shared" si="72"/>
+        <f t="shared" si="82"/>
         <v>800</v>
       </c>
     </row>
@@ -23635,7 +23630,7 @@
         <v>4</v>
       </c>
       <c r="J350" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
@@ -23647,7 +23642,7 @@
         <v>189</v>
       </c>
       <c r="E351" s="92" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="81"/>
         <v>10th %ile</v>
       </c>
       <c r="F351" s="185">
@@ -23666,7 +23661,7 @@
         <v>4</v>
       </c>
       <c r="J351" s="178">
-        <f t="shared" si="72"/>
+        <f t="shared" si="82"/>
         <v>800</v>
       </c>
     </row>
@@ -23677,7 +23672,7 @@
         <v>123</v>
       </c>
       <c r="E352" s="92" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="81"/>
         <v>10th %ile</v>
       </c>
       <c r="F352" s="185">
@@ -23696,7 +23691,7 @@
         <v>4</v>
       </c>
       <c r="J352" s="178">
-        <f t="shared" si="72"/>
+        <f t="shared" si="82"/>
         <v>800</v>
       </c>
     </row>
@@ -23708,7 +23703,7 @@
         <v>192</v>
       </c>
       <c r="E353" s="92" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="81"/>
         <v>10th %ile</v>
       </c>
       <c r="F353" s="185">
@@ -23727,7 +23722,7 @@
         <v>4</v>
       </c>
       <c r="J353" s="178">
-        <f t="shared" si="72"/>
+        <f t="shared" si="82"/>
         <v>800</v>
       </c>
     </row>
@@ -23739,7 +23734,7 @@
         <v>191</v>
       </c>
       <c r="E354" s="92" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="81"/>
         <v>10th %ile</v>
       </c>
       <c r="F354" s="185">
@@ -23758,7 +23753,7 @@
         <v>4</v>
       </c>
       <c r="J354" s="178">
-        <f t="shared" si="72"/>
+        <f t="shared" si="82"/>
         <v>800</v>
       </c>
     </row>
@@ -23789,24 +23784,34 @@
         <v>4</v>
       </c>
       <c r="J355" s="178">
-        <f t="shared" si="70"/>
+        <f t="shared" si="80"/>
         <v>800</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A108:C108"/>
+    <mergeCell ref="A112:C112"/>
+    <mergeCell ref="A110:C110"/>
     <mergeCell ref="A256:E256"/>
     <mergeCell ref="G256:K256"/>
     <mergeCell ref="A109:C109"/>
     <mergeCell ref="A111:C111"/>
     <mergeCell ref="A113:C113"/>
-    <mergeCell ref="A108:C108"/>
-    <mergeCell ref="A112:C112"/>
-    <mergeCell ref="A110:C110"/>
   </mergeCells>
   <conditionalFormatting sqref="F340:F341 F353:F354">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>$D$327</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F108:F113">
+    <cfRule type="cellIs" dxfId="4" priority="20" operator="lessThan">
+      <formula>curMaxBlocksize/1000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E108:E113">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>curMaxBlocksize*1000/avgTrSize/secondsPerBlock</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23817,23 +23822,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="18" operator="lessThan" id="{CCBBA876-7DF4-468C-8839-EA8CEE01F71E}">
-            <xm:f>'Current Bitcoin'!$C$19</xm:f>
-            <x14:dxf>
-              <font>
-                <color auto="1"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFBD1D7"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F108 F110</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="16" operator="lessThan" id="{E16F959B-687E-48F0-9CC9-FF6B850AFA7F}">
+          <x14:cfRule type="cellIs" priority="18" operator="lessThan" id="{E16F959B-687E-48F0-9CC9-FF6B850AFA7F}">
             <xm:f>'Current Bitcoin'!$B$19</xm:f>
             <x14:dxf>
               <fill>
@@ -23846,23 +23835,7 @@
           <xm:sqref>G113 G108:G110</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" operator="lessThan" id="{321EA6B3-025D-4AB3-8E5D-63B63B669534}">
-            <xm:f>'Current Bitcoin'!$C$19/1000</xm:f>
-            <x14:dxf>
-              <font>
-                <color auto="1"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFBD1D7"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F111:F113 F109</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="21" operator="lessThan" id="{A26EE87F-1C32-41E6-AC03-91370DB0C051}">
+          <x14:cfRule type="cellIs" priority="23" operator="lessThan" id="{A26EE87F-1C32-41E6-AC03-91370DB0C051}">
             <xm:f>'Current Bitcoin'!$C$19*1000/'Current Bitcoin'!$C$10/'Current Bitcoin'!$A$15</xm:f>
             <x14:dxf>
               <fill>
@@ -23875,7 +23848,7 @@
           <xm:sqref>F333:F335 F337:F338 F355 F347:F352</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="lessThan" id="{BF534268-13FE-4670-A168-B3AF843E34D3}">
+          <x14:cfRule type="cellIs" priority="4" operator="lessThan" id="{BF534268-13FE-4670-A168-B3AF843E34D3}">
             <xm:f>'Current Bitcoin'!$C$19/1000</xm:f>
             <x14:dxf>
               <font>

</xml_diff>